<commit_message>
2020 Q3 and region_labels.py fix
</commit_message>
<xml_diff>
--- a/web_files/US Power Sector CO2 Emissions Intensity.xlsx
+++ b/web_files/US Power Sector CO2 Emissions Intensity.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="328">
   <si>
     <t>year</t>
   </si>
@@ -271,6 +271,15 @@
     <t>2019 Q4</t>
   </si>
   <si>
+    <t>2020 Q1</t>
+  </si>
+  <si>
+    <t>2020 Q2</t>
+  </si>
+  <si>
+    <t>2020 Q3</t>
+  </si>
+  <si>
     <t>month</t>
   </si>
   <si>
@@ -959,6 +968,39 @@
   </si>
   <si>
     <t>2019-12-01</t>
+  </si>
+  <si>
+    <t>2020-01-01</t>
+  </si>
+  <si>
+    <t>2020-02-01</t>
+  </si>
+  <si>
+    <t>2020-03-01</t>
+  </si>
+  <si>
+    <t>2020-04-01</t>
+  </si>
+  <si>
+    <t>2020-05-01</t>
+  </si>
+  <si>
+    <t>2020-06-01</t>
+  </si>
+  <si>
+    <t>2020-07-01</t>
+  </si>
+  <si>
+    <t>2020-08-01</t>
+  </si>
+  <si>
+    <t>2020-09-01</t>
+  </si>
+  <si>
+    <t>2020-10-01</t>
+  </si>
+  <si>
+    <t>2020-11-01</t>
   </si>
 </sst>
 </file>
@@ -1343,16 +1385,16 @@
         <v>3736520411.15</v>
       </c>
       <c r="C2" t="n">
-        <v>2353860029437.351</v>
+        <v>2353859942597.416</v>
       </c>
       <c r="D2" t="n">
-        <v>629.9604365637325</v>
+        <v>629.9604133228759</v>
       </c>
       <c r="E2" t="n">
-        <v>0.05146536909547494</v>
+        <v>0.05146533030421997</v>
       </c>
       <c r="F2" t="n">
-        <v>1388.810778448405</v>
+        <v>1388.810727211612</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1603,16 +1645,16 @@
         <v>4104659454.56</v>
       </c>
       <c r="C15" t="n">
-        <v>2094303066176.628</v>
+        <v>2094336942609.711</v>
       </c>
       <c r="D15" t="n">
-        <v>510.2257786209277</v>
+        <v>510.2340317862529</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.1483834452111595</v>
+        <v>-0.1483696698738189</v>
       </c>
       <c r="F15" t="n">
-        <v>1124.843751547697</v>
+        <v>1124.861946475973</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1623,16 +1665,16 @@
         <v>4091519853.68</v>
       </c>
       <c r="C16" t="n">
-        <v>1969404902369.6</v>
+        <v>1969813639028.55</v>
       </c>
       <c r="D16" t="n">
-        <v>481.3382246204368</v>
+        <v>481.4381231113563</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.1965995884265576</v>
+        <v>-0.1964328481083881</v>
       </c>
       <c r="F16" t="n">
-        <v>1061.158249998215</v>
+        <v>1061.378486211296</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1643,16 +1685,16 @@
         <v>4095208935.53</v>
       </c>
       <c r="C17" t="n">
-        <v>1856506247039.617</v>
+        <v>1856972230087.1</v>
       </c>
       <c r="D17" t="n">
-        <v>453.3361487206634</v>
+        <v>453.4499360889803</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.2433377823868001</v>
+        <v>-0.2431478601785445</v>
       </c>
       <c r="F17" t="n">
-        <v>999.4248734695744</v>
+        <v>999.675729101766</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1660,19 +1702,19 @@
         <v>2017</v>
       </c>
       <c r="B18" t="n">
-        <v>4058031422.78</v>
+        <v>4058030988.1</v>
       </c>
       <c r="C18" t="n">
-        <v>1779916488949.637</v>
+        <v>1780344062107.865</v>
       </c>
       <c r="D18" t="n">
-        <v>438.6157482561545</v>
+        <v>438.7211599242702</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.2679075655180652</v>
+        <v>-0.2677316231698014</v>
       </c>
       <c r="F18" t="n">
-        <v>966.9722786055182</v>
+        <v>967.2046691690463</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1680,19 +1722,19 @@
         <v>2018</v>
       </c>
       <c r="B19" t="n">
-        <v>4203722496.77</v>
+        <v>4207602186.04</v>
       </c>
       <c r="C19" t="n">
-        <v>1798006646646.182</v>
+        <v>1798435688364.013</v>
       </c>
       <c r="D19" t="n">
-        <v>427.7177306607918</v>
+        <v>427.4253146675487</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.2860974190838259</v>
+        <v>-0.2865854898775124</v>
       </c>
       <c r="F19" t="n">
-        <v>942.9465090147817</v>
+        <v>942.301848716078</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1700,19 +1742,19 @@
         <v>2019</v>
       </c>
       <c r="B20" t="n">
-        <v>4150964239.09</v>
+        <v>4161408263.33</v>
       </c>
       <c r="C20" t="n">
-        <v>1648274509389.186</v>
+        <v>1655720094900.914</v>
       </c>
       <c r="D20" t="n">
-        <v>397.0823197818082</v>
+        <v>397.8749476447645</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.3372309057881187</v>
+        <v>-0.3359079326296378</v>
       </c>
       <c r="F20" t="n">
-        <v>875.4076821909745</v>
+        <v>877.1551095776477</v>
       </c>
     </row>
   </sheetData>
@@ -1726,7 +1768,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H77"/>
+  <dimension ref="A1:H80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1771,19 +1813,19 @@
         <v>916130656.04</v>
       </c>
       <c r="D2" t="n">
-        <v>583241791738.2903</v>
+        <v>583241769147.9152</v>
       </c>
       <c r="E2" t="n">
-        <v>636.6360386403496</v>
+        <v>636.6360139818852</v>
       </c>
       <c r="F2" t="n">
-        <v>0.06260759961349352</v>
+        <v>0.06260755845611317</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
       </c>
       <c r="H2" t="n">
-        <v>1403.527810786515</v>
+        <v>1403.527756424464</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1797,19 +1839,19 @@
         <v>906257293.04</v>
       </c>
       <c r="D3" t="n">
-        <v>568057984771.8798</v>
+        <v>568057964188.5997</v>
       </c>
       <c r="E3" t="n">
-        <v>626.8175595766568</v>
+        <v>626.8175368642545</v>
       </c>
       <c r="F3" t="n">
-        <v>0.04621960107667165</v>
+        <v>0.04621956316745877</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
       </c>
       <c r="H3" t="n">
-        <v>1381.881991842697</v>
+        <v>1381.881941770935</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1823,19 +1865,19 @@
         <v>1035003699.03</v>
       </c>
       <c r="D4" t="n">
-        <v>661654488827.2874</v>
+        <v>661654467247.4973</v>
       </c>
       <c r="E4" t="n">
-        <v>639.2774146096159</v>
+        <v>639.2773937596518</v>
       </c>
       <c r="F4" t="n">
-        <v>0.06701631355368</v>
+        <v>0.06701627875305749</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
       </c>
       <c r="H4" t="n">
-        <v>1409.350988248359</v>
+        <v>1409.350942282528</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1849,19 +1891,19 @@
         <v>879128763.04</v>
       </c>
       <c r="D5" t="n">
-        <v>540905764099.8939</v>
+        <v>540905742013.4038</v>
       </c>
       <c r="E5" t="n">
-        <v>615.2747889051641</v>
+        <v>615.2747637820069</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02695359178458238</v>
+        <v>0.02695354985158447</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
       <c r="H5" t="n">
-        <v>1356.434799620325</v>
+        <v>1356.434744233813</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3201,19 +3243,19 @@
         <v>972455551.6799999</v>
       </c>
       <c r="D57" t="n">
-        <v>476330945536.1271</v>
+        <v>476364821969.2092</v>
       </c>
       <c r="E57" t="n">
-        <v>489.8228455925051</v>
+        <v>489.8576815631812</v>
       </c>
       <c r="F57" t="n">
-        <v>-0.1824379290520509</v>
+        <v>-0.1823797844216285</v>
       </c>
       <c r="G57" t="s">
         <v>63</v>
       </c>
       <c r="H57" t="n">
-        <v>1079.863445393237</v>
+        <v>1079.94024477419</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3227,19 +3269,19 @@
         <v>1021760431.8</v>
       </c>
       <c r="D58" t="n">
-        <v>498659053509.0075</v>
+        <v>498753744965.5725</v>
       </c>
       <c r="E58" t="n">
-        <v>488.0391117030605</v>
+        <v>488.1317865156857</v>
       </c>
       <c r="F58" t="n">
-        <v>-0.1854151547690556</v>
+        <v>-0.1852604714740309</v>
       </c>
       <c r="G58" t="s">
         <v>64</v>
       </c>
       <c r="H58" t="n">
-        <v>1075.931025660567</v>
+        <v>1076.135336552481</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -3253,19 +3295,19 @@
         <v>982642600.02</v>
       </c>
       <c r="D59" t="n">
-        <v>465590894128.4685</v>
+        <v>465714921076.3663</v>
       </c>
       <c r="E59" t="n">
-        <v>473.8150922003506</v>
+        <v>473.9413099603941</v>
       </c>
       <c r="F59" t="n">
-        <v>-0.2091564296942231</v>
+        <v>-0.2089457599506208</v>
       </c>
       <c r="G59" t="s">
         <v>65</v>
       </c>
       <c r="H59" t="n">
-        <v>1044.572752264893</v>
+        <v>1044.851011938685</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -3279,19 +3321,19 @@
         <v>1146880730.57</v>
       </c>
       <c r="D60" t="n">
-        <v>582823928019.964</v>
+        <v>582925062991.5507</v>
       </c>
       <c r="E60" t="n">
-        <v>508.1818121839926</v>
+        <v>508.2699948248643</v>
       </c>
       <c r="F60" t="n">
-        <v>-0.1517950244140596</v>
+        <v>-0.1516478389915308</v>
       </c>
       <c r="G60" t="s">
         <v>66</v>
       </c>
       <c r="H60" t="n">
-        <v>1120.33762314083</v>
+        <v>1120.532030590896</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -3305,19 +3347,19 @@
         <v>940236091.2899996</v>
       </c>
       <c r="D61" t="n">
-        <v>422331026712.1603</v>
+        <v>422419909995.0613</v>
       </c>
       <c r="E61" t="n">
-        <v>449.1755109429208</v>
+        <v>449.270043883875</v>
       </c>
       <c r="F61" t="n">
-        <v>-0.2502822923635057</v>
+        <v>-0.2501245076711934</v>
       </c>
       <c r="G61" t="s">
         <v>67</v>
       </c>
       <c r="H61" t="n">
-        <v>990.2523314247632</v>
+        <v>990.4607387463907</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -3331,19 +3373,19 @@
         <v>974403112.76</v>
       </c>
       <c r="D62" t="n">
-        <v>415639262441.1859</v>
+        <v>415739548171.6349</v>
       </c>
       <c r="E62" t="n">
-        <v>426.5578147260698</v>
+        <v>426.6607348924115</v>
       </c>
       <c r="F62" t="n">
-        <v>-0.2880334318326182</v>
+        <v>-0.287861648043655</v>
       </c>
       <c r="G62" t="s">
         <v>68</v>
       </c>
       <c r="H62" t="n">
-        <v>940.3893583450937</v>
+        <v>940.6162561438106</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -3357,19 +3399,19 @@
         <v>982883128.3099999</v>
       </c>
       <c r="D63" t="n">
-        <v>424304061915.073</v>
+        <v>424470029824.5038</v>
       </c>
       <c r="E63" t="n">
-        <v>431.6933007535034</v>
+        <v>431.862158987662</v>
       </c>
       <c r="F63" t="n">
-        <v>-0.2794618051114635</v>
+        <v>-0.2791799642605159</v>
       </c>
       <c r="G63" t="s">
         <v>69</v>
       </c>
       <c r="H63" t="n">
-        <v>951.7110508411736</v>
+        <v>952.0833157041997</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3383,19 +3425,19 @@
         <v>1178666326.37</v>
       </c>
       <c r="D64" t="n">
-        <v>582953948950.9454</v>
+        <v>583063507517.9319</v>
       </c>
       <c r="E64" t="n">
-        <v>494.5877691664434</v>
+        <v>494.6807204661754</v>
       </c>
       <c r="F64" t="n">
-        <v>-0.1744848071834591</v>
+        <v>-0.1743296624045048</v>
       </c>
       <c r="G64" t="s">
         <v>70</v>
       </c>
       <c r="H64" t="n">
-        <v>1090.368195904341</v>
+        <v>1090.57311633973</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -3409,19 +3451,19 @@
         <v>959256368.09</v>
       </c>
       <c r="D65" t="n">
-        <v>433608973732.4133</v>
+        <v>433699144573.0292</v>
       </c>
       <c r="E65" t="n">
-        <v>452.0261612605016</v>
+        <v>452.1201620340335</v>
       </c>
       <c r="F65" t="n">
-        <v>-0.2455242791386006</v>
+        <v>-0.2453673826855851</v>
       </c>
       <c r="G65" t="s">
         <v>71</v>
       </c>
       <c r="H65" t="n">
-        <v>996.5368751149017</v>
+        <v>996.7441092202304</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -3432,22 +3474,22 @@
         <v>1</v>
       </c>
       <c r="C66" t="n">
-        <v>955342907.37</v>
+        <v>959282668.98</v>
       </c>
       <c r="D66" t="n">
-        <v>409142786134.1847</v>
+        <v>409254135032.1849</v>
       </c>
       <c r="E66" t="n">
-        <v>428.2679894076248</v>
+        <v>426.625173440632</v>
       </c>
       <c r="F66" t="n">
-        <v>-0.2851789836031904</v>
+        <v>-0.2879210035727496</v>
       </c>
       <c r="G66" t="s">
         <v>72</v>
       </c>
       <c r="H66" t="n">
-        <v>944.1596094480497</v>
+        <v>940.5378573672174</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -3458,22 +3500,22 @@
         <v>2</v>
       </c>
       <c r="C67" t="n">
-        <v>981830373.5599999</v>
+        <v>984400726.63</v>
       </c>
       <c r="D67" t="n">
-        <v>417506819519.4294</v>
+        <v>417630905920.5593</v>
       </c>
       <c r="E67" t="n">
-        <v>425.2331469494058</v>
+        <v>424.248880179394</v>
       </c>
       <c r="F67" t="n">
-        <v>-0.2902444314635101</v>
+        <v>-0.2918872686363715</v>
       </c>
       <c r="G67" t="s">
         <v>73</v>
       </c>
       <c r="H67" t="n">
-        <v>937.46899576466</v>
+        <v>935.299081243492</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -3484,22 +3526,22 @@
         <v>3</v>
       </c>
       <c r="C68" t="n">
-        <v>1131773341.65</v>
+        <v>1132268520.22</v>
       </c>
       <c r="D68" t="n">
-        <v>529307839523.9713</v>
+        <v>529405339850.721</v>
       </c>
       <c r="E68" t="n">
-        <v>467.6800734255669</v>
+        <v>467.5616520256674</v>
       </c>
       <c r="F68" t="n">
-        <v>-0.2193963739923487</v>
+        <v>-0.2195940308509816</v>
       </c>
       <c r="G68" t="s">
         <v>74</v>
       </c>
       <c r="H68" t="n">
-        <v>1031.047489874005</v>
+        <v>1030.786418055786</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -3510,22 +3552,22 @@
         <v>4</v>
       </c>
       <c r="C69" t="n">
-        <v>989084800.2000002</v>
+        <v>982079072.27</v>
       </c>
       <c r="D69" t="n">
-        <v>423959043772.0515</v>
+        <v>424053681304.3992</v>
       </c>
       <c r="E69" t="n">
-        <v>428.6377100187202</v>
+        <v>431.7917907813999</v>
       </c>
       <c r="F69" t="n">
-        <v>-0.284561883867645</v>
+        <v>-0.2792974156553583</v>
       </c>
       <c r="G69" t="s">
         <v>75</v>
       </c>
       <c r="H69" t="n">
-        <v>944.9746955072707</v>
+        <v>951.9281819566744</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3536,22 +3578,22 @@
         <v>1</v>
       </c>
       <c r="C70" t="n">
-        <v>1007401406.23</v>
+        <v>1007451607.32</v>
       </c>
       <c r="D70" t="n">
-        <v>419548425578.4994</v>
+        <v>419640230123.809</v>
       </c>
       <c r="E70" t="n">
-        <v>416.4659915937344</v>
+        <v>416.5363646995675</v>
       </c>
       <c r="F70" t="n">
-        <v>-0.3048776682620815</v>
+        <v>-0.3047602086893774</v>
       </c>
       <c r="G70" t="s">
         <v>76</v>
       </c>
       <c r="H70" t="n">
-        <v>918.1409250675467</v>
+        <v>918.2960696166666</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -3562,22 +3604,22 @@
         <v>2</v>
       </c>
       <c r="C71" t="n">
-        <v>1020316668.44</v>
+        <v>1020356356.43</v>
       </c>
       <c r="D71" t="n">
-        <v>415249700035.8303</v>
+        <v>415356885261.8722</v>
       </c>
       <c r="E71" t="n">
-        <v>406.9811979752532</v>
+        <v>407.0704148059738</v>
       </c>
       <c r="F71" t="n">
-        <v>-0.3207087132674637</v>
+        <v>-0.3205598016812776</v>
       </c>
       <c r="G71" t="s">
         <v>77</v>
       </c>
       <c r="H71" t="n">
-        <v>897.2307490562433</v>
+        <v>897.42743648125</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -3588,22 +3630,22 @@
         <v>3</v>
       </c>
       <c r="C72" t="n">
-        <v>1184301080.04</v>
+        <v>1184368755.68</v>
       </c>
       <c r="D72" t="n">
-        <v>538431152830.669</v>
+        <v>538558569559.6967</v>
       </c>
       <c r="E72" t="n">
-        <v>454.6404304659448</v>
+        <v>454.7220339753777</v>
       </c>
       <c r="F72" t="n">
-        <v>-0.2411608090292548</v>
+        <v>-0.2410246048183471</v>
       </c>
       <c r="G72" t="s">
         <v>78</v>
       </c>
       <c r="H72" t="n">
-        <v>1002.300293005222</v>
+        <v>1002.480196102118</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3614,22 +3656,22 @@
         <v>4</v>
       </c>
       <c r="C73" t="n">
-        <v>991703342.0599999</v>
+        <v>995425466.61</v>
       </c>
       <c r="D73" t="n">
-        <v>424777368201.1837</v>
+        <v>424880003418.6351</v>
       </c>
       <c r="E73" t="n">
-        <v>428.3310846959753</v>
+        <v>426.8325632310749</v>
       </c>
       <c r="F73" t="n">
-        <v>-0.2850736714172131</v>
+        <v>-0.2875748497988012</v>
       </c>
       <c r="G73" t="s">
         <v>79</v>
       </c>
       <c r="H73" t="n">
-        <v>944.2987093207473</v>
+        <v>940.995068899228</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3640,22 +3682,22 @@
         <v>1</v>
       </c>
       <c r="C74" t="n">
-        <v>1001779191.56</v>
+        <v>1007788097.36</v>
       </c>
       <c r="D74" t="n">
-        <v>404430216314.0046</v>
+        <v>405162129362.0672</v>
       </c>
       <c r="E74" t="n">
-        <v>403.7119354457882</v>
+        <v>402.0310722297964</v>
       </c>
       <c r="F74" t="n">
-        <v>-0.3261654310749576</v>
+        <v>-0.3289709556114545</v>
       </c>
       <c r="G74" t="s">
         <v>80</v>
       </c>
       <c r="H74" t="n">
-        <v>890.0233328837846</v>
+        <v>886.3177018378093</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -3666,22 +3708,22 @@
         <v>2</v>
       </c>
       <c r="C75" t="n">
-        <v>983904422.5400002</v>
+        <v>990197617.6799999</v>
       </c>
       <c r="D75" t="n">
-        <v>366151132876.4085</v>
+        <v>368851959498.5653</v>
       </c>
       <c r="E75" t="n">
-        <v>372.1409564672657</v>
+        <v>372.5033800452612</v>
       </c>
       <c r="F75" t="n">
-        <v>-0.37886047212457</v>
+        <v>-0.3782555518484895</v>
       </c>
       <c r="G75" t="s">
         <v>81</v>
       </c>
       <c r="H75" t="n">
-        <v>820.4219526277341</v>
+        <v>821.2209516477827</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -3692,22 +3734,22 @@
         <v>3</v>
       </c>
       <c r="C76" t="n">
-        <v>1182927572.9</v>
+        <v>1182237725.04</v>
       </c>
       <c r="D76" t="n">
-        <v>501538054468.6464</v>
+        <v>504677843173.925</v>
       </c>
       <c r="E76" t="n">
-        <v>423.9803568354598</v>
+        <v>426.8835552146248</v>
       </c>
       <c r="F76" t="n">
-        <v>-0.2923354602696122</v>
+        <v>-0.2874897392082117</v>
       </c>
       <c r="G76" t="s">
         <v>82</v>
       </c>
       <c r="H76" t="n">
-        <v>934.7070946794548</v>
+        <v>941.1074858261617</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3718,22 +3760,100 @@
         <v>4</v>
       </c>
       <c r="C77" t="n">
-        <v>982353052.09</v>
+        <v>981184823.2500002</v>
       </c>
       <c r="D77" t="n">
-        <v>376155105730.1261</v>
+        <v>377028162866.3561</v>
       </c>
       <c r="E77" t="n">
-        <v>382.9123398454754</v>
+        <v>384.2580459179112</v>
       </c>
       <c r="F77" t="n">
-        <v>-0.3608819834099183</v>
+        <v>-0.3586358688128399</v>
       </c>
       <c r="G77" t="s">
         <v>83</v>
       </c>
       <c r="H77" t="n">
-        <v>844.1685444233351</v>
+        <v>847.135288030627</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B78" t="n">
+        <v>1</v>
+      </c>
+      <c r="C78" t="n">
+        <v>973085219.9299999</v>
+      </c>
+      <c r="D78" t="n">
+        <v>336644951803.2552</v>
+      </c>
+      <c r="E78" t="n">
+        <v>345.9562892420379</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-0.4225652338692876</v>
+      </c>
+      <c r="G78" t="s">
+        <v>84</v>
+      </c>
+      <c r="H78" t="n">
+        <v>762.695235262997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B79" t="n">
+        <v>2</v>
+      </c>
+      <c r="C79" t="n">
+        <v>944544519.86</v>
+      </c>
+      <c r="D79" t="n">
+        <v>314159373200.5373</v>
+      </c>
+      <c r="E79" t="n">
+        <v>332.6040928670064</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-0.4448513510202138</v>
+      </c>
+      <c r="G79" t="s">
+        <v>85</v>
+      </c>
+      <c r="H79" t="n">
+        <v>733.2589831346022</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B80" t="n">
+        <v>3</v>
+      </c>
+      <c r="C80" t="n">
+        <v>1160166124.9</v>
+      </c>
+      <c r="D80" t="n">
+        <v>472407748264.4694</v>
+      </c>
+      <c r="E80" t="n">
+        <v>407.1897447490017</v>
+      </c>
+      <c r="F80" t="n">
+        <v>-0.3203606283756104</v>
+      </c>
+      <c r="G80" t="s">
+        <v>86</v>
+      </c>
+      <c r="H80" t="n">
+        <v>897.6905112736492</v>
       </c>
     </row>
   </sheetData>
@@ -3747,7 +3867,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I229"/>
+  <dimension ref="A1:I240"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3760,7 +3880,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -3775,7 +3895,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -3795,22 +3915,22 @@
         <v>332483912.02</v>
       </c>
       <c r="D2" t="n">
-        <v>214591031919.6448</v>
+        <v>214591023941.9348</v>
       </c>
       <c r="E2" t="n">
-        <v>645.4177906410595</v>
+        <v>645.4177666467857</v>
       </c>
       <c r="F2" t="n">
-        <v>0.07726519963532781</v>
+        <v>0.07726515958654644</v>
       </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>1422.888061247279</v>
+        <v>1422.888008349504</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3824,22 +3944,22 @@
         <v>282940199.01</v>
       </c>
       <c r="D3" t="n">
-        <v>179938999258.3465</v>
+        <v>179938992004.0915</v>
       </c>
       <c r="E3" t="n">
-        <v>635.9612380564803</v>
+        <v>635.9612124176523</v>
       </c>
       <c r="F3" t="n">
-        <v>0.06148129166810185</v>
+        <v>0.06148124887439917</v>
       </c>
       <c r="G3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>1402.040145419316</v>
+        <v>1402.040088895956</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3853,22 +3973,22 @@
         <v>300706545.0100001</v>
       </c>
       <c r="D4" t="n">
-        <v>188711760560.2989</v>
+        <v>188711753201.8889</v>
       </c>
       <c r="E4" t="n">
-        <v>627.5612010840114</v>
+        <v>627.5611766136095</v>
       </c>
       <c r="F4" t="n">
-        <v>0.04746081123309126</v>
+        <v>0.04746077038960551</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>1383.521423909811</v>
+        <v>1383.521369962364</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3882,22 +4002,22 @@
         <v>278078103</v>
       </c>
       <c r="D5" t="n">
-        <v>174479653321.1478</v>
+        <v>174479645962.7378</v>
       </c>
       <c r="E5" t="n">
-        <v>627.4483730966325</v>
+        <v>627.448346634966</v>
       </c>
       <c r="F5" t="n">
-        <v>0.04727249032512958</v>
+        <v>0.04727244615802906</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="H5" t="n">
         <v>2</v>
       </c>
       <c r="I5" t="n">
-        <v>1383.272683328836</v>
+        <v>1383.272624991446</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3911,22 +4031,22 @@
         <v>300485702.02</v>
       </c>
       <c r="D6" t="n">
-        <v>188798233302.9063</v>
+        <v>188798226769.2913</v>
       </c>
       <c r="E6" t="n">
-        <v>628.3102058890646</v>
+        <v>628.3101841455508</v>
       </c>
       <c r="F6" t="n">
-        <v>0.04871097325611524</v>
+        <v>0.04871093696407162</v>
       </c>
       <c r="G6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H6" t="n">
         <v>2</v>
       </c>
       <c r="I6" t="n">
-        <v>1385.172679903032</v>
+        <v>1385.172631967281</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3940,22 +4060,22 @@
         <v>327693488.02</v>
       </c>
       <c r="D7" t="n">
-        <v>204780098147.8257</v>
+        <v>204780091456.5706</v>
       </c>
       <c r="E7" t="n">
-        <v>624.913541569454</v>
+        <v>624.9135211502048</v>
       </c>
       <c r="F7" t="n">
-        <v>0.04304160944337442</v>
+        <v>0.04304157536165719</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H7" t="n">
         <v>2</v>
       </c>
       <c r="I7" t="n">
-        <v>1377.684393744019</v>
+        <v>1377.684348727741</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3969,22 +4089,22 @@
         <v>357589591</v>
       </c>
       <c r="D8" t="n">
-        <v>229405343975.5568</v>
+        <v>229405336724.1168</v>
       </c>
       <c r="E8" t="n">
-        <v>641.5324991256715</v>
+        <v>641.5324788470052</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0707802694077172</v>
+        <v>0.07078023556064666</v>
       </c>
       <c r="G8" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H8" t="n">
         <v>3</v>
       </c>
       <c r="I8" t="n">
-        <v>1414.322547572456</v>
+        <v>1414.322502866107</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3998,22 +4118,22 @@
         <v>370485240.02</v>
       </c>
       <c r="D9" t="n">
-        <v>238687749752.5028</v>
+        <v>238687742503.8778</v>
       </c>
       <c r="E9" t="n">
-        <v>644.2571092430502</v>
+        <v>644.2570896778309</v>
       </c>
       <c r="F9" t="n">
-        <v>0.07532790925370161</v>
+        <v>0.07532787659744344</v>
       </c>
       <c r="G9" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H9" t="n">
         <v>3</v>
       </c>
       <c r="I9" t="n">
-        <v>1420.329223037229</v>
+        <v>1420.329179903746</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -4027,22 +4147,22 @@
         <v>306928868.01</v>
       </c>
       <c r="D10" t="n">
-        <v>193561395099.2277</v>
+        <v>193561388019.5027</v>
       </c>
       <c r="E10" t="n">
-        <v>630.6392629477958</v>
+        <v>630.6392398814579</v>
       </c>
       <c r="F10" t="n">
-        <v>0.05259839649377376</v>
+        <v>0.05259835799380738</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H10" t="n">
         <v>3</v>
       </c>
       <c r="I10" t="n">
-        <v>1390.307319094711</v>
+        <v>1390.307268242662</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4056,22 +4176,22 @@
         <v>294730111.03</v>
       </c>
       <c r="D11" t="n">
-        <v>182854818134.092</v>
+        <v>182854810905.172</v>
       </c>
       <c r="E11" t="n">
-        <v>620.4144445746149</v>
+        <v>620.4144200473618</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0355321780446675</v>
+        <v>0.03553213710629145</v>
       </c>
       <c r="G11" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H11" t="n">
         <v>4</v>
       </c>
       <c r="I11" t="n">
-        <v>1367.765684509196</v>
+        <v>1367.765630436414</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -4085,22 +4205,22 @@
         <v>278902324</v>
       </c>
       <c r="D12" t="n">
-        <v>171520217078.9825</v>
+        <v>171520209703.6825</v>
       </c>
       <c r="E12" t="n">
-        <v>614.9831045473197</v>
+        <v>614.9830781032947</v>
       </c>
       <c r="F12" t="n">
-        <v>0.02646674216168697</v>
+        <v>0.02646669802403197</v>
       </c>
       <c r="G12" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H12" t="n">
         <v>4</v>
       </c>
       <c r="I12" t="n">
-        <v>1355.791752285021</v>
+        <v>1355.791693986524</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -4114,22 +4234,22 @@
         <v>305496328.01</v>
       </c>
       <c r="D13" t="n">
-        <v>186530728886.8195</v>
+        <v>186530721404.5494</v>
       </c>
       <c r="E13" t="n">
-        <v>610.5825562679548</v>
+        <v>610.5825317757783</v>
       </c>
       <c r="F13" t="n">
-        <v>0.01912179817437256</v>
+        <v>0.01912175729454257</v>
       </c>
       <c r="G13" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H13" t="n">
         <v>4</v>
       </c>
       <c r="I13" t="n">
-        <v>1346.090303548333</v>
+        <v>1346.090249552881</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -4152,7 +4272,7 @@
         <v>0.01111774538231211</v>
       </c>
       <c r="G14" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H14" t="n">
         <v>1</v>
@@ -4181,7 +4301,7 @@
         <v>0.005018273091192093</v>
       </c>
       <c r="G15" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H15" t="n">
         <v>1</v>
@@ -4210,7 +4330,7 @@
         <v>0.01544195713902331</v>
       </c>
       <c r="G16" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H16" t="n">
         <v>1</v>
@@ -4239,7 +4359,7 @@
         <v>0.003355439027818183</v>
       </c>
       <c r="G17" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H17" t="n">
         <v>2</v>
@@ -4268,7 +4388,7 @@
         <v>0.00536957613039397</v>
       </c>
       <c r="G18" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H18" t="n">
         <v>2</v>
@@ -4297,7 +4417,7 @@
         <v>0.0145689414097139</v>
       </c>
       <c r="G19" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H19" t="n">
         <v>2</v>
@@ -4326,7 +4446,7 @@
         <v>0.03912865348530959</v>
       </c>
       <c r="G20" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H20" t="n">
         <v>3</v>
@@ -4355,7 +4475,7 @@
         <v>0.04573043199637251</v>
       </c>
       <c r="G21" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="H21" t="n">
         <v>3</v>
@@ -4384,7 +4504,7 @@
         <v>0.05004182162970362</v>
       </c>
       <c r="G22" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="H22" t="n">
         <v>3</v>
@@ -4413,7 +4533,7 @@
         <v>0.0547357353567896</v>
       </c>
       <c r="G23" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H23" t="n">
         <v>4</v>
@@ -4442,7 +4562,7 @@
         <v>0.03397983951034167</v>
       </c>
       <c r="G24" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H24" t="n">
         <v>4</v>
@@ -4471,7 +4591,7 @@
         <v>0.03489294255166995</v>
       </c>
       <c r="G25" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H25" t="n">
         <v>4</v>
@@ -4500,7 +4620,7 @@
         <v>0.05407231572896915</v>
       </c>
       <c r="G26" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H26" t="n">
         <v>1</v>
@@ -4529,7 +4649,7 @@
         <v>0.0446998960634503</v>
       </c>
       <c r="G27" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="H27" t="n">
         <v>1</v>
@@ -4558,7 +4678,7 @@
         <v>0.02564607186253928</v>
       </c>
       <c r="G28" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="H28" t="n">
         <v>1</v>
@@ -4587,7 +4707,7 @@
         <v>-0.005255460204990879</v>
       </c>
       <c r="G29" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H29" t="n">
         <v>2</v>
@@ -4616,7 +4736,7 @@
         <v>-0.005159282455205773</v>
       </c>
       <c r="G30" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="H30" t="n">
         <v>2</v>
@@ -4645,7 +4765,7 @@
         <v>0.01662217479072057</v>
       </c>
       <c r="G31" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="H31" t="n">
         <v>2</v>
@@ -4674,7 +4794,7 @@
         <v>0.03768728145702852</v>
       </c>
       <c r="G32" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H32" t="n">
         <v>3</v>
@@ -4703,7 +4823,7 @@
         <v>0.04140058597533856</v>
       </c>
       <c r="G33" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H33" t="n">
         <v>3</v>
@@ -4732,7 +4852,7 @@
         <v>0.04146258828233757</v>
       </c>
       <c r="G34" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="H34" t="n">
         <v>3</v>
@@ -4761,7 +4881,7 @@
         <v>0.05070299868862761</v>
       </c>
       <c r="G35" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H35" t="n">
         <v>4</v>
@@ -4790,7 +4910,7 @@
         <v>0.04234991120899041</v>
       </c>
       <c r="G36" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H36" t="n">
         <v>4</v>
@@ -4819,7 +4939,7 @@
         <v>0.03310887154716038</v>
       </c>
       <c r="G37" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H37" t="n">
         <v>4</v>
@@ -4848,7 +4968,7 @@
         <v>0.03014022625659499</v>
       </c>
       <c r="G38" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H38" t="n">
         <v>1</v>
@@ -4877,7 +4997,7 @@
         <v>0.01239560014339367</v>
       </c>
       <c r="G39" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H39" t="n">
         <v>1</v>
@@ -4906,7 +5026,7 @@
         <v>-0.01037094285092945</v>
       </c>
       <c r="G40" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="H40" t="n">
         <v>1</v>
@@ -4935,7 +5055,7 @@
         <v>-0.02234624922534889</v>
       </c>
       <c r="G41" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H41" t="n">
         <v>2</v>
@@ -4964,7 +5084,7 @@
         <v>-0.01332959283944984</v>
       </c>
       <c r="G42" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H42" t="n">
         <v>2</v>
@@ -4993,7 +5113,7 @@
         <v>-0.007522138257441214</v>
       </c>
       <c r="G43" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H43" t="n">
         <v>2</v>
@@ -5022,7 +5142,7 @@
         <v>0.002774173076043244</v>
       </c>
       <c r="G44" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H44" t="n">
         <v>3</v>
@@ -5051,7 +5171,7 @@
         <v>0.005812723595943646</v>
       </c>
       <c r="G45" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H45" t="n">
         <v>3</v>
@@ -5080,7 +5200,7 @@
         <v>-0.0001281622510707689</v>
       </c>
       <c r="G46" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H46" t="n">
         <v>3</v>
@@ -5109,7 +5229,7 @@
         <v>0.005798551352125575</v>
       </c>
       <c r="G47" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H47" t="n">
         <v>4</v>
@@ -5138,7 +5258,7 @@
         <v>0.0142697616731208</v>
       </c>
       <c r="G48" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H48" t="n">
         <v>4</v>
@@ -5167,7 +5287,7 @@
         <v>0.006630546904983436</v>
       </c>
       <c r="G49" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="H49" t="n">
         <v>4</v>
@@ -5196,7 +5316,7 @@
         <v>0.01135874913719794</v>
       </c>
       <c r="G50" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="H50" t="n">
         <v>1</v>
@@ -5225,7 +5345,7 @@
         <v>0.00158584139446698</v>
       </c>
       <c r="G51" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H51" t="n">
         <v>1</v>
@@ -5254,7 +5374,7 @@
         <v>0.0004943352228414668</v>
       </c>
       <c r="G52" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H52" t="n">
         <v>1</v>
@@ -5283,7 +5403,7 @@
         <v>-0.03023291224285088</v>
       </c>
       <c r="G53" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H53" t="n">
         <v>2</v>
@@ -5312,7 +5432,7 @@
         <v>-0.03619156271650293</v>
       </c>
       <c r="G54" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="H54" t="n">
         <v>2</v>
@@ -5341,7 +5461,7 @@
         <v>-0.007018965988378289</v>
       </c>
       <c r="G55" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="H55" t="n">
         <v>2</v>
@@ -5370,7 +5490,7 @@
         <v>-0.0008959033638951873</v>
       </c>
       <c r="G56" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="H56" t="n">
         <v>3</v>
@@ -5399,7 +5519,7 @@
         <v>0.007925452227224232</v>
       </c>
       <c r="G57" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H57" t="n">
         <v>3</v>
@@ -5428,7 +5548,7 @@
         <v>0.01721030590351288</v>
       </c>
       <c r="G58" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H58" t="n">
         <v>3</v>
@@ -5457,7 +5577,7 @@
         <v>0.02231843704751483</v>
       </c>
       <c r="G59" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="H59" t="n">
         <v>4</v>
@@ -5486,7 +5606,7 @@
         <v>0.002897748801680964</v>
       </c>
       <c r="G60" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="H60" t="n">
         <v>4</v>
@@ -5515,7 +5635,7 @@
         <v>0.00389971424966281</v>
       </c>
       <c r="G61" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H61" t="n">
         <v>4</v>
@@ -5544,7 +5664,7 @@
         <v>-0.02748121131636642</v>
       </c>
       <c r="G62" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="H62" t="n">
         <v>1</v>
@@ -5573,7 +5693,7 @@
         <v>-0.01857254232013877</v>
       </c>
       <c r="G63" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="H63" t="n">
         <v>1</v>
@@ -5602,7 +5722,7 @@
         <v>-0.02435619078134472</v>
       </c>
       <c r="G64" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="H64" t="n">
         <v>1</v>
@@ -5631,7 +5751,7 @@
         <v>-0.06369815302300276</v>
       </c>
       <c r="G65" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="H65" t="n">
         <v>2</v>
@@ -5660,7 +5780,7 @@
         <v>-0.05404582225952413</v>
       </c>
       <c r="G66" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H66" t="n">
         <v>2</v>
@@ -5689,7 +5809,7 @@
         <v>-0.04243926553323214</v>
       </c>
       <c r="G67" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H67" t="n">
         <v>2</v>
@@ -5718,7 +5838,7 @@
         <v>-0.01354297585931169</v>
       </c>
       <c r="G68" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H68" t="n">
         <v>3</v>
@@ -5747,7 +5867,7 @@
         <v>-0.004118886890496862</v>
       </c>
       <c r="G69" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H69" t="n">
         <v>3</v>
@@ -5776,7 +5896,7 @@
         <v>-0.01455882450582037</v>
       </c>
       <c r="G70" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H70" t="n">
         <v>3</v>
@@ -5805,7 +5925,7 @@
         <v>0.00439522235340898</v>
       </c>
       <c r="G71" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="H71" t="n">
         <v>4</v>
@@ -5834,7 +5954,7 @@
         <v>-0.003746313420402704</v>
       </c>
       <c r="G72" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H72" t="n">
         <v>4</v>
@@ -5863,7 +5983,7 @@
         <v>-0.01605853233048685</v>
       </c>
       <c r="G73" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H73" t="n">
         <v>4</v>
@@ -5892,7 +6012,7 @@
         <v>-0.03511432398711213</v>
       </c>
       <c r="G74" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="H74" t="n">
         <v>1</v>
@@ -5921,7 +6041,7 @@
         <v>-0.008437620703637254</v>
       </c>
       <c r="G75" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="H75" t="n">
         <v>1</v>
@@ -5950,7 +6070,7 @@
         <v>-0.03117857292861368</v>
       </c>
       <c r="G76" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H76" t="n">
         <v>1</v>
@@ -5979,7 +6099,7 @@
         <v>-0.03928361585166878</v>
       </c>
       <c r="G77" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H77" t="n">
         <v>2</v>
@@ -6008,7 +6128,7 @@
         <v>-0.03788195719455209</v>
       </c>
       <c r="G78" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H78" t="n">
         <v>2</v>
@@ -6037,7 +6157,7 @@
         <v>-0.0177532915761511</v>
       </c>
       <c r="G79" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="H79" t="n">
         <v>2</v>
@@ -6066,7 +6186,7 @@
         <v>-0.01310236048309173</v>
       </c>
       <c r="G80" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H80" t="n">
         <v>3</v>
@@ -6095,7 +6215,7 @@
         <v>-0.008678539752206496</v>
       </c>
       <c r="G81" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H81" t="n">
         <v>3</v>
@@ -6124,7 +6244,7 @@
         <v>-0.004141764801333879</v>
       </c>
       <c r="G82" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="H82" t="n">
         <v>3</v>
@@ -6153,7 +6273,7 @@
         <v>1.642574651693381e-05</v>
       </c>
       <c r="G83" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H83" t="n">
         <v>4</v>
@@ -6182,7 +6302,7 @@
         <v>-0.01470502580322882</v>
       </c>
       <c r="G84" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H84" t="n">
         <v>4</v>
@@ -6211,7 +6331,7 @@
         <v>-0.01552034206631986</v>
       </c>
       <c r="G85" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="H85" t="n">
         <v>4</v>
@@ -6240,7 +6360,7 @@
         <v>-0.01703554138701916</v>
       </c>
       <c r="G86" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H86" t="n">
         <v>1</v>
@@ -6269,7 +6389,7 @@
         <v>-0.01289961080171436</v>
       </c>
       <c r="G87" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H87" t="n">
         <v>1</v>
@@ -6298,7 +6418,7 @@
         <v>-0.03539719528073028</v>
       </c>
       <c r="G88" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H88" t="n">
         <v>1</v>
@@ -6327,7 +6447,7 @@
         <v>-0.04508011761521417</v>
       </c>
       <c r="G89" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="H89" t="n">
         <v>2</v>
@@ -6356,7 +6476,7 @@
         <v>-0.04957830570333151</v>
       </c>
       <c r="G90" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H90" t="n">
         <v>2</v>
@@ -6385,7 +6505,7 @@
         <v>-0.04880070678863985</v>
       </c>
       <c r="G91" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H91" t="n">
         <v>2</v>
@@ -6414,7 +6534,7 @@
         <v>-0.0274894180589785</v>
       </c>
       <c r="G92" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H92" t="n">
         <v>3</v>
@@ -6443,7 +6563,7 @@
         <v>-0.02085837505734224</v>
       </c>
       <c r="G93" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H93" t="n">
         <v>3</v>
@@ -6472,7 +6592,7 @@
         <v>-0.01669978454361145</v>
       </c>
       <c r="G94" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H94" t="n">
         <v>3</v>
@@ -6501,7 +6621,7 @@
         <v>-0.02999219344874965</v>
       </c>
       <c r="G95" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H95" t="n">
         <v>4</v>
@@ -6530,7 +6650,7 @@
         <v>-0.03080314982097817</v>
       </c>
       <c r="G96" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H96" t="n">
         <v>4</v>
@@ -6559,7 +6679,7 @@
         <v>-0.04600766838125035</v>
       </c>
       <c r="G97" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H97" t="n">
         <v>4</v>
@@ -6588,7 +6708,7 @@
         <v>-0.05120162818415125</v>
       </c>
       <c r="G98" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="H98" t="n">
         <v>1</v>
@@ -6617,7 +6737,7 @@
         <v>-0.06946387564298999</v>
       </c>
       <c r="G99" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="H99" t="n">
         <v>1</v>
@@ -6646,7 +6766,7 @@
         <v>-0.1036546461764051</v>
       </c>
       <c r="G100" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H100" t="n">
         <v>1</v>
@@ -6675,7 +6795,7 @@
         <v>-0.1132003468526878</v>
       </c>
       <c r="G101" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="H101" t="n">
         <v>2</v>
@@ -6704,7 +6824,7 @@
         <v>-0.1231526853843904</v>
       </c>
       <c r="G102" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="H102" t="n">
         <v>2</v>
@@ -6733,7 +6853,7 @@
         <v>-0.09824854233094853</v>
       </c>
       <c r="G103" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="H103" t="n">
         <v>2</v>
@@ -6762,7 +6882,7 @@
         <v>-0.07814990231786137</v>
       </c>
       <c r="G104" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="H104" t="n">
         <v>3</v>
@@ -6791,7 +6911,7 @@
         <v>-0.06154336099479781</v>
       </c>
       <c r="G105" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="H105" t="n">
         <v>3</v>
@@ -6820,7 +6940,7 @@
         <v>-0.08482641466001017</v>
       </c>
       <c r="G106" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="H106" t="n">
         <v>3</v>
@@ -6849,7 +6969,7 @@
         <v>-0.06247971785652189</v>
       </c>
       <c r="G107" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H107" t="n">
         <v>4</v>
@@ -6878,7 +6998,7 @@
         <v>-0.07639133784549447</v>
       </c>
       <c r="G108" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="H108" t="n">
         <v>4</v>
@@ -6907,7 +7027,7 @@
         <v>-0.06443636967118098</v>
       </c>
       <c r="G109" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="H109" t="n">
         <v>4</v>
@@ -6936,7 +7056,7 @@
         <v>-0.0488799844984841</v>
       </c>
       <c r="G110" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="H110" t="n">
         <v>1</v>
@@ -6965,7 +7085,7 @@
         <v>-0.05825045169669583</v>
       </c>
       <c r="G111" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="H111" t="n">
         <v>1</v>
@@ -6994,7 +7114,7 @@
         <v>-0.07735581168612655</v>
       </c>
       <c r="G112" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="H112" t="n">
         <v>1</v>
@@ -7023,7 +7143,7 @@
         <v>-0.1010225664365227</v>
       </c>
       <c r="G113" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="H113" t="n">
         <v>2</v>
@@ -7052,7 +7172,7 @@
         <v>-0.08979818195601069</v>
       </c>
       <c r="G114" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="H114" t="n">
         <v>2</v>
@@ -7081,7 +7201,7 @@
         <v>-0.06524048333304372</v>
       </c>
       <c r="G115" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="H115" t="n">
         <v>2</v>
@@ -7110,7 +7230,7 @@
         <v>-0.04074387693241805</v>
       </c>
       <c r="G116" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="H116" t="n">
         <v>3</v>
@@ -7139,7 +7259,7 @@
         <v>-0.03675707967139325</v>
       </c>
       <c r="G117" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="H117" t="n">
         <v>3</v>
@@ -7168,7 +7288,7 @@
         <v>-0.07201037569984288</v>
       </c>
       <c r="G118" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="H118" t="n">
         <v>3</v>
@@ -7197,7 +7317,7 @@
         <v>-0.08798764407113459</v>
       </c>
       <c r="G119" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="H119" t="n">
         <v>4</v>
@@ -7226,7 +7346,7 @@
         <v>-0.09297937195930114</v>
       </c>
       <c r="G120" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="H120" t="n">
         <v>4</v>
@@ -7255,7 +7375,7 @@
         <v>-0.06888446180263902</v>
       </c>
       <c r="G121" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H121" t="n">
         <v>4</v>
@@ -7284,7 +7404,7 @@
         <v>-0.06178402409839879</v>
       </c>
       <c r="G122" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="H122" t="n">
         <v>1</v>
@@ -7313,7 +7433,7 @@
         <v>-0.1000963753988781</v>
       </c>
       <c r="G123" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="H123" t="n">
         <v>1</v>
@@ -7342,7 +7462,7 @@
         <v>-0.129184632154868</v>
       </c>
       <c r="G124" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="H124" t="n">
         <v>1</v>
@@ -7371,7 +7491,7 @@
         <v>-0.1349292609291222</v>
       </c>
       <c r="G125" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="H125" t="n">
         <v>2</v>
@@ -7400,7 +7520,7 @@
         <v>-0.1059778059250063</v>
       </c>
       <c r="G126" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="H126" t="n">
         <v>2</v>
@@ -7429,7 +7549,7 @@
         <v>-0.081007853314257</v>
       </c>
       <c r="G127" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="H127" t="n">
         <v>2</v>
@@ -7458,7 +7578,7 @@
         <v>-0.06182654921614888</v>
       </c>
       <c r="G128" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="H128" t="n">
         <v>3</v>
@@ -7487,7 +7607,7 @@
         <v>-0.05965103240997342</v>
       </c>
       <c r="G129" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="H129" t="n">
         <v>3</v>
@@ -7516,7 +7636,7 @@
         <v>-0.0903372091951556</v>
       </c>
       <c r="G130" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="H130" t="n">
         <v>3</v>
@@ -7545,7 +7665,7 @@
         <v>-0.1209466228210752</v>
       </c>
       <c r="G131" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="H131" t="n">
         <v>4</v>
@@ -7574,7 +7694,7 @@
         <v>-0.1459020669822017</v>
       </c>
       <c r="G132" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="H132" t="n">
         <v>4</v>
@@ -7603,7 +7723,7 @@
         <v>-0.1448500018406984</v>
       </c>
       <c r="G133" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H133" t="n">
         <v>4</v>
@@ -7632,7 +7752,7 @@
         <v>-0.1655768065392497</v>
       </c>
       <c r="G134" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="H134" t="n">
         <v>1</v>
@@ -7661,7 +7781,7 @@
         <v>-0.1688920478560091</v>
       </c>
       <c r="G135" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H135" t="n">
         <v>1</v>
@@ -7690,7 +7810,7 @@
         <v>-0.20286842192788</v>
       </c>
       <c r="G136" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H136" t="n">
         <v>1</v>
@@ -7719,7 +7839,7 @@
         <v>-0.2134075015003669</v>
       </c>
       <c r="G137" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H137" t="n">
         <v>2</v>
@@ -7748,7 +7868,7 @@
         <v>-0.1749832923810191</v>
       </c>
       <c r="G138" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="H138" t="n">
         <v>2</v>
@@ -7777,7 +7897,7 @@
         <v>-0.1347935101828394</v>
       </c>
       <c r="G139" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="H139" t="n">
         <v>2</v>
@@ -7806,7 +7926,7 @@
         <v>-0.08586343302838688</v>
       </c>
       <c r="G140" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="H140" t="n">
         <v>3</v>
@@ -7835,7 +7955,7 @@
         <v>-0.09583413286254644</v>
       </c>
       <c r="G141" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="H141" t="n">
         <v>3</v>
@@ -7864,7 +7984,7 @@
         <v>-0.1212332640457878</v>
       </c>
       <c r="G142" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="H142" t="n">
         <v>3</v>
@@ -7893,7 +8013,7 @@
         <v>-0.1291033474036325</v>
       </c>
       <c r="G143" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="H143" t="n">
         <v>4</v>
@@ -7922,7 +8042,7 @@
         <v>-0.103972413775247</v>
       </c>
       <c r="G144" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="H144" t="n">
         <v>4</v>
@@ -7951,7 +8071,7 @@
         <v>-0.1496729265861562</v>
       </c>
       <c r="G145" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H145" t="n">
         <v>4</v>
@@ -7980,7 +8100,7 @@
         <v>-0.1485961495296913</v>
       </c>
       <c r="G146" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="H146" t="n">
         <v>1</v>
@@ -8009,7 +8129,7 @@
         <v>-0.1453195655542535</v>
       </c>
       <c r="G147" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="H147" t="n">
         <v>1</v>
@@ -8038,7 +8158,7 @@
         <v>-0.1386143662583348</v>
       </c>
       <c r="G148" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="H148" t="n">
         <v>1</v>
@@ -8067,7 +8187,7 @@
         <v>-0.1821179183493233</v>
       </c>
       <c r="G149" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="H149" t="n">
         <v>2</v>
@@ -8096,7 +8216,7 @@
         <v>-0.1753852982577576</v>
       </c>
       <c r="G150" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="H150" t="n">
         <v>2</v>
@@ -8125,7 +8245,7 @@
         <v>-0.1318627511501101</v>
       </c>
       <c r="G151" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="H151" t="n">
         <v>2</v>
@@ -8154,7 +8274,7 @@
         <v>-0.1101448680751284</v>
       </c>
       <c r="G152" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="H152" t="n">
         <v>3</v>
@@ -8183,7 +8303,7 @@
         <v>-0.1060645126133002</v>
       </c>
       <c r="G153" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="H153" t="n">
         <v>3</v>
@@ -8212,7 +8332,7 @@
         <v>-0.1135082142199412</v>
       </c>
       <c r="G154" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="H154" t="n">
         <v>3</v>
@@ -8241,7 +8361,7 @@
         <v>-0.1418981805314145</v>
       </c>
       <c r="G155" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="H155" t="n">
         <v>4</v>
@@ -8270,7 +8390,7 @@
         <v>-0.1588733260713331</v>
       </c>
       <c r="G156" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="H156" t="n">
         <v>4</v>
@@ -8299,7 +8419,7 @@
         <v>-0.1335324447797183</v>
       </c>
       <c r="G157" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="H157" t="n">
         <v>4</v>
@@ -8328,7 +8448,7 @@
         <v>-0.1164250865344272</v>
       </c>
       <c r="G158" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="H158" t="n">
         <v>1</v>
@@ -8357,7 +8477,7 @@
         <v>-0.09235435026425724</v>
       </c>
       <c r="G159" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="H159" t="n">
         <v>1</v>
@@ -8386,7 +8506,7 @@
         <v>-0.1404967846693579</v>
       </c>
       <c r="G160" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="H160" t="n">
         <v>1</v>
@@ -8415,7 +8535,7 @@
         <v>-0.1979602327171737</v>
       </c>
       <c r="G161" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="H161" t="n">
         <v>2</v>
@@ -8444,7 +8564,7 @@
         <v>-0.1819517134786032</v>
       </c>
       <c r="G162" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="H162" t="n">
         <v>2</v>
@@ -8473,7 +8593,7 @@
         <v>-0.1479617441739821</v>
       </c>
       <c r="G163" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="H163" t="n">
         <v>2</v>
@@ -8502,7 +8622,7 @@
         <v>-0.1235469123516771</v>
       </c>
       <c r="G164" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="H164" t="n">
         <v>3</v>
@@ -8531,7 +8651,7 @@
         <v>-0.1112892814595854</v>
       </c>
       <c r="G165" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="H165" t="n">
         <v>3</v>
@@ -8560,7 +8680,7 @@
         <v>-0.1428458470250424</v>
       </c>
       <c r="G166" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="H166" t="n">
         <v>3</v>
@@ -8580,22 +8700,22 @@
         <v>315466648.72</v>
       </c>
       <c r="D167" t="n">
-        <v>154932143967.0348</v>
+        <v>154941566540.2584</v>
       </c>
       <c r="E167" t="n">
-        <v>491.1205181139402</v>
+        <v>491.1503867966103</v>
       </c>
       <c r="F167" t="n">
-        <v>-0.1802719871332877</v>
+        <v>-0.1802221333906949</v>
       </c>
       <c r="G167" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="H167" t="n">
         <v>4</v>
       </c>
       <c r="I167" t="n">
-        <v>1082.724294233993</v>
+        <v>1082.790142731807</v>
       </c>
     </row>
     <row r="168" spans="1:9">
@@ -8609,22 +8729,22 @@
         <v>318278457.49</v>
       </c>
       <c r="D168" t="n">
-        <v>156252560431.6124</v>
+        <v>156260369449.2323</v>
       </c>
       <c r="E168" t="n">
-        <v>490.9303685327861</v>
+        <v>490.9549037076813</v>
       </c>
       <c r="F168" t="n">
-        <v>-0.1805893653175784</v>
+        <v>-0.1805484137193039</v>
       </c>
       <c r="G168" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="H168" t="n">
         <v>4</v>
       </c>
       <c r="I168" t="n">
-        <v>1082.30509046738</v>
+        <v>1082.359180713954</v>
       </c>
     </row>
     <row r="169" spans="1:9">
@@ -8638,22 +8758,22 @@
         <v>338710445.47</v>
       </c>
       <c r="D169" t="n">
-        <v>165146241137.4799</v>
+        <v>165162885979.7187</v>
       </c>
       <c r="E169" t="n">
-        <v>487.5735110805937</v>
+        <v>487.622652884342</v>
       </c>
       <c r="F169" t="n">
-        <v>-0.1861922875887348</v>
+        <v>-0.1861102651285657</v>
       </c>
       <c r="G169" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="H169" t="n">
         <v>4</v>
       </c>
       <c r="I169" t="n">
-        <v>1074.904562528277</v>
+        <v>1075.01290054882</v>
       </c>
     </row>
     <row r="170" spans="1:9">
@@ -8667,22 +8787,22 @@
         <v>361191037.38</v>
       </c>
       <c r="D170" t="n">
-        <v>177351526240.8069</v>
+        <v>177376622712.9249</v>
       </c>
       <c r="E170" t="n">
-        <v>491.0186241809203</v>
+        <v>491.0881067248396</v>
       </c>
       <c r="F170" t="n">
-        <v>-0.1804420580388129</v>
+        <v>-0.1803260849007435</v>
       </c>
       <c r="G170" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="H170" t="n">
         <v>1</v>
       </c>
       <c r="I170" t="n">
-        <v>1082.499658869257</v>
+        <v>1082.652840085581</v>
       </c>
     </row>
     <row r="171" spans="1:9">
@@ -8696,22 +8816,22 @@
         <v>335258891.09</v>
       </c>
       <c r="D171" t="n">
-        <v>169353608681.8348</v>
+        <v>169384015346.2678</v>
       </c>
       <c r="E171" t="n">
-        <v>505.1427812435614</v>
+        <v>505.2334773152871</v>
       </c>
       <c r="F171" t="n">
-        <v>-0.156867463259431</v>
+        <v>-0.15671608267583</v>
       </c>
       <c r="G171" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="H171" t="n">
         <v>1</v>
       </c>
       <c r="I171" t="n">
-        <v>1113.637775529556</v>
+        <v>1113.837724089282</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -8725,22 +8845,22 @@
         <v>325310503.33</v>
       </c>
       <c r="D172" t="n">
-        <v>151953918586.3658</v>
+        <v>151993106906.3797</v>
       </c>
       <c r="E172" t="n">
-        <v>467.1042497272872</v>
+        <v>467.2247140824578</v>
       </c>
       <c r="F172" t="n">
-        <v>-0.2203574798686929</v>
+        <v>-0.2201564131185913</v>
       </c>
       <c r="G172" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="H172" t="n">
         <v>1</v>
       </c>
       <c r="I172" t="n">
-        <v>1029.778028948777</v>
+        <v>1030.043604666187</v>
       </c>
     </row>
     <row r="173" spans="1:9">
@@ -8754,22 +8874,22 @@
         <v>295382039.3200001</v>
       </c>
       <c r="D173" t="n">
-        <v>130280851166.6377</v>
+        <v>130317918718.6098</v>
       </c>
       <c r="E173" t="n">
-        <v>441.0588113839206</v>
+        <v>441.1843015865661</v>
       </c>
       <c r="F173" t="n">
-        <v>-0.2638298550393369</v>
+        <v>-0.2636203996599449</v>
       </c>
       <c r="G173" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="H173" t="n">
         <v>2</v>
       </c>
       <c r="I173" t="n">
-        <v>972.3582555769914</v>
+        <v>972.6349112777436</v>
       </c>
     </row>
     <row r="174" spans="1:9">
@@ -8783,22 +8903,22 @@
         <v>323464197.98</v>
       </c>
       <c r="D174" t="n">
-        <v>152433162012.342</v>
+        <v>152473724386.401</v>
       </c>
       <c r="E174" t="n">
-        <v>471.2520364364005</v>
+        <v>471.3774363239687</v>
       </c>
       <c r="F174" t="n">
-        <v>-0.2134344195780869</v>
+        <v>-0.2132251149433617</v>
       </c>
       <c r="G174" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="H174" t="n">
         <v>2</v>
       </c>
       <c r="I174" t="n">
-        <v>1038.922239527689</v>
+        <v>1039.198696119821</v>
       </c>
     </row>
     <row r="175" spans="1:9">
@@ -8812,22 +8932,22 @@
         <v>363796362.72</v>
       </c>
       <c r="D175" t="n">
-        <v>182876880949.4888</v>
+        <v>182923277971.3556</v>
       </c>
       <c r="E175" t="n">
-        <v>502.6902401721977</v>
+        <v>502.8177758669471</v>
       </c>
       <c r="F175" t="n">
-        <v>-0.1609609933498121</v>
+        <v>-0.1607481238447302</v>
       </c>
       <c r="G175" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="H175" t="n">
         <v>2</v>
       </c>
       <c r="I175" t="n">
-        <v>1108.230903483627</v>
+        <v>1108.512068676272</v>
       </c>
     </row>
     <row r="176" spans="1:9">
@@ -8841,22 +8961,22 @@
         <v>401883971.8900002</v>
       </c>
       <c r="D176" t="n">
-        <v>205967765565.5143</v>
+        <v>205996928296.2257</v>
       </c>
       <c r="E176" t="n">
-        <v>512.5055487952874</v>
+        <v>512.5781138457776</v>
       </c>
       <c r="F176" t="n">
-        <v>-0.1445782865873711</v>
+        <v>-0.1444571684453917</v>
       </c>
       <c r="G176" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="H176" t="n">
         <v>3</v>
       </c>
       <c r="I176" t="n">
-        <v>1129.869732874091</v>
+        <v>1130.029709784401</v>
       </c>
     </row>
     <row r="177" spans="1:9">
@@ -8870,22 +8990,22 @@
         <v>393563699.96</v>
       </c>
       <c r="D177" t="n">
-        <v>201013924204.8849</v>
+        <v>201050121274.9237</v>
       </c>
       <c r="E177" t="n">
-        <v>510.7532128225114</v>
+        <v>510.8451854054566</v>
       </c>
       <c r="F177" t="n">
-        <v>-0.1475031061211891</v>
+        <v>-0.1473495949159449</v>
       </c>
       <c r="G177" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="H177" t="n">
         <v>3</v>
       </c>
       <c r="I177" t="n">
-        <v>1126.006532988509</v>
+        <v>1126.209295744869</v>
       </c>
     </row>
     <row r="178" spans="1:9">
@@ -8899,22 +9019,22 @@
         <v>351433058.72</v>
       </c>
       <c r="D178" t="n">
-        <v>175842238249.5647</v>
+        <v>175878013420.4012</v>
       </c>
       <c r="E178" t="n">
-        <v>500.3577036549224</v>
+        <v>500.4595016217013</v>
       </c>
       <c r="F178" t="n">
-        <v>-0.1648542241429136</v>
+        <v>-0.1646843134143985</v>
       </c>
       <c r="G178" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="H178" t="n">
         <v>3</v>
       </c>
       <c r="I178" t="n">
-        <v>1103.088593477642</v>
+        <v>1103.313017275203</v>
       </c>
     </row>
     <row r="179" spans="1:9">
@@ -8928,22 +9048,22 @@
         <v>313291653.9699998</v>
       </c>
       <c r="D179" t="n">
-        <v>147818692467.4064</v>
+        <v>147841586374.8496</v>
       </c>
       <c r="E179" t="n">
-        <v>471.8245462152056</v>
+        <v>471.8976215976904</v>
       </c>
       <c r="F179" t="n">
-        <v>-0.2124788449563445</v>
+        <v>-0.2123568750205254</v>
       </c>
       <c r="G179" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="H179" t="n">
         <v>4</v>
       </c>
       <c r="I179" t="n">
-        <v>1040.184394586042</v>
+        <v>1040.345496574268</v>
       </c>
     </row>
     <row r="180" spans="1:9">
@@ -8957,22 +9077,22 @@
         <v>301619345.3299999</v>
       </c>
       <c r="D180" t="n">
-        <v>134985954680.743</v>
+        <v>135018144430.7121</v>
       </c>
       <c r="E180" t="n">
-        <v>447.5374566344729</v>
+        <v>447.6441797292201</v>
       </c>
       <c r="F180" t="n">
-        <v>-0.2530163646608481</v>
+        <v>-0.2528382334137154</v>
       </c>
       <c r="G180" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="H180" t="n">
         <v>4</v>
       </c>
       <c r="I180" t="n">
-        <v>986.6410768963588</v>
+        <v>986.8763586310383</v>
       </c>
     </row>
     <row r="181" spans="1:9">
@@ -8986,22 +9106,22 @@
         <v>325325091.9899999</v>
       </c>
       <c r="D181" t="n">
-        <v>139526379564.011</v>
+        <v>139560179189.4995</v>
       </c>
       <c r="E181" t="n">
-        <v>428.8829327935757</v>
+        <v>428.9868277169024</v>
       </c>
       <c r="F181" t="n">
-        <v>-0.2841525831552374</v>
+        <v>-0.2839791724018593</v>
       </c>
       <c r="G181" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="H181" t="n">
         <v>4</v>
       </c>
       <c r="I181" t="n">
-        <v>945.5153136367172</v>
+        <v>945.7443603846832</v>
       </c>
     </row>
     <row r="182" spans="1:9">
@@ -9015,22 +9135,22 @@
         <v>353691242.9900001</v>
       </c>
       <c r="D182" t="n">
-        <v>161014969060.6654</v>
+        <v>161038384325.4114</v>
       </c>
       <c r="E182" t="n">
-        <v>455.2416047948855</v>
+        <v>455.3078073520878</v>
       </c>
       <c r="F182" t="n">
-        <v>-0.2401573904794831</v>
+        <v>-0.2400468919589356</v>
       </c>
       <c r="G182" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="H182" t="n">
         <v>1</v>
       </c>
       <c r="I182" t="n">
-        <v>1003.625641930805</v>
+        <v>1003.771592088413</v>
       </c>
     </row>
     <row r="183" spans="1:9">
@@ -9044,22 +9164,22 @@
         <v>314822845.6500002</v>
       </c>
       <c r="D183" t="n">
-        <v>135657677633.6077</v>
+        <v>135697119874.8574</v>
       </c>
       <c r="E183" t="n">
-        <v>430.9016308950565</v>
+        <v>431.0269148183635</v>
       </c>
       <c r="F183" t="n">
-        <v>-0.280783179267044</v>
+        <v>-0.2805740681879732</v>
       </c>
       <c r="G183" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="H183" t="n">
         <v>1</v>
       </c>
       <c r="I183" t="n">
-        <v>949.9657354712416</v>
+        <v>950.2419364085644</v>
       </c>
     </row>
     <row r="184" spans="1:9">
@@ -9073,22 +9193,22 @@
         <v>305889024.1199999</v>
       </c>
       <c r="D184" t="n">
-        <v>118966615746.9128</v>
+        <v>119004043971.3661</v>
       </c>
       <c r="E184" t="n">
-        <v>388.9208384941668</v>
+        <v>389.0431973285873</v>
       </c>
       <c r="F184" t="n">
-        <v>-0.3508532135338012</v>
+        <v>-0.3506489847131821</v>
       </c>
       <c r="G184" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="H184" t="n">
         <v>1</v>
       </c>
       <c r="I184" t="n">
-        <v>857.4148805442403</v>
+        <v>857.6846328306036</v>
       </c>
     </row>
     <row r="185" spans="1:9">
@@ -9102,22 +9222,22 @@
         <v>294568958.4599999</v>
       </c>
       <c r="D185" t="n">
-        <v>116606267223.6425</v>
+        <v>116646161120.9464</v>
       </c>
       <c r="E185" t="n">
-        <v>395.8538870940698</v>
+        <v>395.9893185309476</v>
       </c>
       <c r="F185" t="n">
-        <v>-0.3392812796758305</v>
+        <v>-0.3390552314075603</v>
       </c>
       <c r="G185" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="H185" t="n">
         <v>2</v>
       </c>
       <c r="I185" t="n">
-        <v>872.6994794875862</v>
+        <v>872.9980516333271</v>
       </c>
     </row>
     <row r="186" spans="1:9">
@@ -9131,22 +9251,22 @@
         <v>318633901.01</v>
       </c>
       <c r="D186" t="n">
-        <v>132149850300.7968</v>
+        <v>132223162145.6396</v>
       </c>
       <c r="E186" t="n">
-        <v>414.738826853987</v>
+        <v>414.968908601756</v>
       </c>
       <c r="F186" t="n">
-        <v>-0.3077604745546056</v>
+        <v>-0.3073764456921587</v>
       </c>
       <c r="G186" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="H186" t="n">
         <v>2</v>
       </c>
       <c r="I186" t="n">
-        <v>914.3332176822996</v>
+        <v>914.8404559034312</v>
       </c>
     </row>
     <row r="187" spans="1:9">
@@ -9160,22 +9280,22 @@
         <v>369680268.84</v>
       </c>
       <c r="D187" t="n">
-        <v>175547944390.6337</v>
+        <v>175600706557.9177</v>
       </c>
       <c r="E187" t="n">
-        <v>474.8642521319198</v>
+        <v>475.0069759171238</v>
       </c>
       <c r="F187" t="n">
-        <v>-0.2074052795097685</v>
+        <v>-0.2071670596013775</v>
       </c>
       <c r="G187" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="H187" t="n">
         <v>2</v>
       </c>
       <c r="I187" t="n">
-        <v>1046.88573025003</v>
+        <v>1047.200379106891</v>
       </c>
     </row>
     <row r="188" spans="1:9">
@@ -9189,22 +9309,22 @@
         <v>413857711.4400001</v>
       </c>
       <c r="D188" t="n">
-        <v>205901334506.1659</v>
+        <v>205933255532.0861</v>
       </c>
       <c r="E188" t="n">
-        <v>497.5172113858675</v>
+        <v>497.5943418223383</v>
       </c>
       <c r="F188" t="n">
-        <v>-0.1695952825947526</v>
+        <v>-0.1694665443785963</v>
       </c>
       <c r="G188" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="H188" t="n">
         <v>3</v>
       </c>
       <c r="I188" t="n">
-        <v>1096.826444221284</v>
+        <v>1096.996485981527</v>
       </c>
     </row>
     <row r="189" spans="1:9">
@@ -9218,22 +9338,22 @@
         <v>411613836.8800002</v>
       </c>
       <c r="D189" t="n">
-        <v>206237885617.5125</v>
+        <v>206275812361.3413</v>
       </c>
       <c r="E189" t="n">
-        <v>501.0470181973937</v>
+        <v>501.1391597641504</v>
       </c>
       <c r="F189" t="n">
-        <v>-0.1637036909859808</v>
+        <v>-0.1635498977302847</v>
       </c>
       <c r="G189" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="H189" t="n">
         <v>3</v>
       </c>
       <c r="I189" t="n">
-        <v>1104.608256317974</v>
+        <v>1104.811391616046</v>
       </c>
     </row>
     <row r="190" spans="1:9">
@@ -9247,22 +9367,22 @@
         <v>353194778.05</v>
       </c>
       <c r="D190" t="n">
-        <v>170814728827.2671</v>
+        <v>170854439624.5045</v>
       </c>
       <c r="E190" t="n">
-        <v>483.6275603233457</v>
+        <v>483.7399934613913</v>
       </c>
       <c r="F190" t="n">
-        <v>-0.1927784640032953</v>
+        <v>-0.1925908021373558</v>
       </c>
       <c r="G190" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="H190" t="n">
         <v>3</v>
       </c>
       <c r="I190" t="n">
-        <v>1066.205319488848</v>
+        <v>1066.453189584983</v>
       </c>
     </row>
     <row r="191" spans="1:9">
@@ -9276,22 +9396,22 @@
         <v>314473312.79</v>
       </c>
       <c r="D191" t="n">
-        <v>144952646041.3123</v>
+        <v>144981418325.4933</v>
       </c>
       <c r="E191" t="n">
-        <v>460.9378288901395</v>
+        <v>461.0293224541743</v>
       </c>
       <c r="F191" t="n">
-        <v>-0.2306498372695747</v>
+        <v>-0.2304971255935805</v>
       </c>
       <c r="G191" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H191" t="n">
         <v>4</v>
       </c>
       <c r="I191" t="n">
-        <v>1016.183537571202</v>
+        <v>1016.385244282473</v>
       </c>
     </row>
     <row r="192" spans="1:9">
@@ -9305,22 +9425,22 @@
         <v>298296665.97</v>
       </c>
       <c r="D192" t="n">
-        <v>128449629426.9714</v>
+        <v>128477773481.6743</v>
       </c>
       <c r="E192" t="n">
-        <v>430.6103422553497</v>
+        <v>430.7046914650915</v>
       </c>
       <c r="F192" t="n">
-        <v>-0.2812693683977985</v>
+        <v>-0.2811118903707875</v>
       </c>
       <c r="G192" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="H192" t="n">
         <v>4</v>
       </c>
       <c r="I192" t="n">
-        <v>949.323560536144</v>
+        <v>949.5315628039407</v>
       </c>
     </row>
     <row r="193" spans="1:9">
@@ -9334,22 +9454,22 @@
         <v>346486389.33</v>
       </c>
       <c r="D193" t="n">
-        <v>160206698264.1296</v>
+        <v>160239952765.8615</v>
       </c>
       <c r="E193" t="n">
-        <v>462.3751558435557</v>
+        <v>462.4711322015194</v>
       </c>
       <c r="F193" t="n">
-        <v>-0.2282507984921106</v>
+        <v>-0.2280906045961236</v>
       </c>
       <c r="G193" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="H193" t="n">
         <v>4</v>
       </c>
       <c r="I193" t="n">
-        <v>1019.352268572703</v>
+        <v>1019.56385805147</v>
       </c>
     </row>
     <row r="194" spans="1:9">
@@ -9360,25 +9480,25 @@
         <v>1</v>
       </c>
       <c r="C194" t="n">
-        <v>344422637.41</v>
+        <v>345564690.4</v>
       </c>
       <c r="D194" t="n">
-        <v>156037863543.1925</v>
+        <v>156071783779.8932</v>
       </c>
       <c r="E194" t="n">
-        <v>453.0418346383123</v>
+        <v>451.6427404641259</v>
       </c>
       <c r="F194" t="n">
-        <v>-0.2438290212762095</v>
+        <v>-0.2461642458186973</v>
       </c>
       <c r="G194" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="H194" t="n">
         <v>1</v>
       </c>
       <c r="I194" t="n">
-        <v>998.776028643623</v>
+        <v>995.691585627212</v>
       </c>
     </row>
     <row r="195" spans="1:9">
@@ -9389,25 +9509,25 @@
         <v>2</v>
       </c>
       <c r="C195" t="n">
-        <v>291027018.9400001</v>
+        <v>292424145.15</v>
       </c>
       <c r="D195" t="n">
-        <v>122156558115.3555</v>
+        <v>122189464127.116</v>
       </c>
       <c r="E195" t="n">
-        <v>419.7430141032372</v>
+        <v>417.8501199497001</v>
       </c>
       <c r="F195" t="n">
-        <v>-0.2994079982915608</v>
+        <v>-0.3025674231288796</v>
       </c>
       <c r="G195" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="H195" t="n">
         <v>1</v>
       </c>
       <c r="I195" t="n">
-        <v>925.3654488919972</v>
+        <v>921.1923744411087</v>
       </c>
     </row>
     <row r="196" spans="1:9">
@@ -9418,25 +9538,25 @@
         <v>3</v>
       </c>
       <c r="C196" t="n">
-        <v>319893251.02</v>
+        <v>321293833.43</v>
       </c>
       <c r="D196" t="n">
-        <v>130948364475.6366</v>
+        <v>130992887125.1756</v>
       </c>
       <c r="E196" t="n">
-        <v>409.3501943479564</v>
+        <v>407.7043301041597</v>
       </c>
       <c r="F196" t="n">
-        <v>-0.3167546274220137</v>
+        <v>-0.3195017352626656</v>
       </c>
       <c r="G196" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="H196" t="n">
         <v>1</v>
       </c>
       <c r="I196" t="n">
-        <v>902.4534384595047</v>
+        <v>898.8249661476303</v>
       </c>
     </row>
     <row r="197" spans="1:9">
@@ -9447,25 +9567,25 @@
         <v>4</v>
       </c>
       <c r="C197" t="n">
-        <v>296510295.3</v>
+        <v>297545922.2499999</v>
       </c>
       <c r="D197" t="n">
-        <v>119903345616.1091</v>
+        <v>119949787286.8673</v>
       </c>
       <c r="E197" t="n">
-        <v>404.3817281109739</v>
+        <v>403.1303349070426</v>
       </c>
       <c r="F197" t="n">
-        <v>-0.3250474818339568</v>
+        <v>-0.3271361790610914</v>
       </c>
       <c r="G197" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="H197" t="n">
         <v>2</v>
       </c>
       <c r="I197" t="n">
-        <v>891.4999577934531</v>
+        <v>888.7411363360661</v>
       </c>
     </row>
     <row r="198" spans="1:9">
@@ -9476,25 +9596,25 @@
         <v>5</v>
       </c>
       <c r="C198" t="n">
-        <v>324929606.96</v>
+        <v>325858747.93</v>
       </c>
       <c r="D198" t="n">
-        <v>136797466380.1694</v>
+        <v>136836902229.1036</v>
       </c>
       <c r="E198" t="n">
-        <v>421.0064686318648</v>
+        <v>419.9270484476866</v>
       </c>
       <c r="F198" t="n">
-        <v>-0.2972991695379247</v>
+        <v>-0.2991008270333654</v>
       </c>
       <c r="G198" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="H198" t="n">
         <v>2</v>
       </c>
       <c r="I198" t="n">
-        <v>928.1508607458094</v>
+        <v>925.7711710077699</v>
       </c>
     </row>
     <row r="199" spans="1:9">
@@ -9505,25 +9625,25 @@
         <v>6</v>
       </c>
       <c r="C199" t="n">
-        <v>360390471.3</v>
+        <v>360996056.4500001</v>
       </c>
       <c r="D199" t="n">
-        <v>160806007523.1508</v>
+        <v>160844216404.5883</v>
       </c>
       <c r="E199" t="n">
-        <v>446.1993874119136</v>
+        <v>445.5567132403457</v>
       </c>
       <c r="F199" t="n">
-        <v>-0.2552497326111403</v>
+        <v>-0.2563224184431297</v>
       </c>
       <c r="G199" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="H199" t="n">
         <v>2</v>
       </c>
       <c r="I199" t="n">
-        <v>983.6911694883047</v>
+        <v>982.2743300096663</v>
       </c>
     </row>
     <row r="200" spans="1:9">
@@ -9534,25 +9654,25 @@
         <v>7</v>
       </c>
       <c r="C200" t="n">
-        <v>406926547.25</v>
+        <v>406971865.19</v>
       </c>
       <c r="D200" t="n">
-        <v>194767485809.7708</v>
+        <v>194796584412.3592</v>
       </c>
       <c r="E200" t="n">
-        <v>478.6305713549653</v>
+        <v>478.6487742129689</v>
       </c>
       <c r="F200" t="n">
-        <v>-0.2011189256339721</v>
+        <v>-0.2010885432897825</v>
       </c>
       <c r="G200" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="H200" t="n">
         <v>3</v>
       </c>
       <c r="I200" t="n">
-        <v>1055.188957609156</v>
+        <v>1055.229087629912</v>
       </c>
     </row>
     <row r="201" spans="1:9">
@@ -9563,25 +9683,25 @@
         <v>8</v>
       </c>
       <c r="C201" t="n">
-        <v>386791100.23</v>
+        <v>387187231.7</v>
       </c>
       <c r="D201" t="n">
-        <v>182290770412.7428</v>
+        <v>182328043021.456</v>
       </c>
       <c r="E201" t="n">
-        <v>471.2899813474148</v>
+        <v>470.9040693850337</v>
       </c>
       <c r="F201" t="n">
-        <v>-0.2133710858232203</v>
+        <v>-0.2140152105021869</v>
       </c>
       <c r="G201" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="H201" t="n">
         <v>3</v>
       </c>
       <c r="I201" t="n">
-        <v>1039.005892878511</v>
+        <v>1038.155111366246</v>
       </c>
     </row>
     <row r="202" spans="1:9">
@@ -9592,25 +9712,25 @@
         <v>9</v>
       </c>
       <c r="C202" t="n">
-        <v>338055694.17</v>
+        <v>338109423.33</v>
       </c>
       <c r="D202" t="n">
-        <v>152249583301.4578</v>
+        <v>152280712416.9059</v>
       </c>
       <c r="E202" t="n">
-        <v>450.3683444092357</v>
+        <v>450.388844289257</v>
       </c>
       <c r="F202" t="n">
-        <v>-0.2482913370461056</v>
+        <v>-0.2482571207482845</v>
       </c>
       <c r="G202" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="H202" t="n">
         <v>3</v>
       </c>
       <c r="I202" t="n">
-        <v>992.8820520846012</v>
+        <v>992.927246120096</v>
       </c>
     </row>
     <row r="203" spans="1:9">
@@ -9621,25 +9741,25 @@
         <v>10</v>
       </c>
       <c r="C203" t="n">
-        <v>322336627.73</v>
+        <v>320630010.1</v>
       </c>
       <c r="D203" t="n">
-        <v>137490153926.8835</v>
+        <v>137530799218.4129</v>
       </c>
       <c r="E203" t="n">
-        <v>426.542136694592</v>
+        <v>428.9392598513126</v>
       </c>
       <c r="F203" t="n">
-        <v>-0.2880595999952484</v>
+        <v>-0.2840585678058347</v>
       </c>
       <c r="G203" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="H203" t="n">
         <v>4</v>
       </c>
       <c r="I203" t="n">
-        <v>940.3547945568976</v>
+        <v>945.6394922682041</v>
       </c>
     </row>
     <row r="204" spans="1:9">
@@ -9650,25 +9770,25 @@
         <v>11</v>
       </c>
       <c r="C204" t="n">
-        <v>311850496.6700001</v>
+        <v>309587425.1</v>
       </c>
       <c r="D204" t="n">
-        <v>132099496723.1551</v>
+        <v>132144974366.0841</v>
       </c>
       <c r="E204" t="n">
-        <v>423.5988017775795</v>
+        <v>426.8421894829865</v>
       </c>
       <c r="F204" t="n">
-        <v>-0.2929723128503119</v>
+        <v>-0.2875587826461171</v>
       </c>
       <c r="G204" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="H204" t="n">
         <v>4</v>
       </c>
       <c r="I204" t="n">
-        <v>933.8659183988518</v>
+        <v>941.0162909341922</v>
       </c>
     </row>
     <row r="205" spans="1:9">
@@ -9679,25 +9799,25 @@
         <v>12</v>
       </c>
       <c r="C205" t="n">
-        <v>354897675.8000001</v>
+        <v>351861637.07</v>
       </c>
       <c r="D205" t="n">
-        <v>154369393122.0129</v>
+        <v>154377907719.9022</v>
       </c>
       <c r="E205" t="n">
-        <v>434.968735070011</v>
+        <v>438.7460622460241</v>
       </c>
       <c r="F205" t="n">
-        <v>-0.2739947859898487</v>
+        <v>-0.267690058767635</v>
       </c>
       <c r="G205" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="H205" t="n">
         <v>4</v>
       </c>
       <c r="I205" t="n">
-        <v>958.9320733353463</v>
+        <v>967.2595688275846</v>
       </c>
     </row>
     <row r="206" spans="1:9">
@@ -9708,25 +9828,25 @@
         <v>1</v>
       </c>
       <c r="C206" t="n">
-        <v>374820337.71</v>
+        <v>374838323.87</v>
       </c>
       <c r="D206" t="n">
-        <v>170282290084.7661</v>
+        <v>170312386318.6317</v>
       </c>
       <c r="E206" t="n">
-        <v>454.3037635714267</v>
+        <v>454.3622555992937</v>
       </c>
       <c r="F206" t="n">
-        <v>-0.2417227388901801</v>
+        <v>-0.2416251099946168</v>
       </c>
       <c r="G206" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="H206" t="n">
         <v>1</v>
       </c>
       <c r="I206" t="n">
-        <v>1001.558077169567</v>
+        <v>1001.687028694203</v>
       </c>
     </row>
     <row r="207" spans="1:9">
@@ -9737,25 +9857,25 @@
         <v>2</v>
       </c>
       <c r="C207" t="n">
-        <v>308632286.96</v>
+        <v>308647892.4299998</v>
       </c>
       <c r="D207" t="n">
-        <v>123351014780.9323</v>
+        <v>123384032535.0363</v>
       </c>
       <c r="E207" t="n">
-        <v>399.6698336260556</v>
+        <v>399.7566014905457</v>
       </c>
       <c r="F207" t="n">
-        <v>-0.3329120929843783</v>
+        <v>-0.3327672689615248</v>
       </c>
       <c r="G207" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="H207" t="n">
         <v>1</v>
       </c>
       <c r="I207" t="n">
-        <v>881.1121152120022</v>
+        <v>881.3034036460573</v>
       </c>
     </row>
     <row r="208" spans="1:9">
@@ -9766,25 +9886,25 @@
         <v>3</v>
       </c>
       <c r="C208" t="n">
-        <v>323948781.5599999</v>
+        <v>323965391.02</v>
       </c>
       <c r="D208" t="n">
-        <v>125915120712.801</v>
+        <v>125943811270.1409</v>
       </c>
       <c r="E208" t="n">
-        <v>388.6883602600607</v>
+        <v>388.756993065243</v>
       </c>
       <c r="F208" t="n">
-        <v>-0.3512412423655233</v>
+        <v>-0.3511266875242277</v>
       </c>
       <c r="G208" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="H208" t="n">
         <v>1</v>
       </c>
       <c r="I208" t="n">
-        <v>856.9023590293299</v>
+        <v>857.0536669116347</v>
       </c>
     </row>
     <row r="209" spans="1:9">
@@ -9795,25 +9915,25 @@
         <v>4</v>
       </c>
       <c r="C209" t="n">
-        <v>303466559.1799999</v>
+        <v>303479515.33</v>
       </c>
       <c r="D209" t="n">
-        <v>116115687046.2829</v>
+        <v>116143375558.0651</v>
       </c>
       <c r="E209" t="n">
-        <v>382.6309144573962</v>
+        <v>382.7058160145411</v>
       </c>
       <c r="F209" t="n">
-        <v>-0.3613517098123629</v>
+        <v>-0.3612266918130441</v>
       </c>
       <c r="G209" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="H209" t="n">
         <v>2</v>
       </c>
       <c r="I209" t="n">
-        <v>843.5481140127756</v>
+        <v>843.7132419856572</v>
       </c>
     </row>
     <row r="210" spans="1:9">
@@ -9824,25 +9944,25 @@
         <v>5</v>
       </c>
       <c r="C210" t="n">
-        <v>341935300.77</v>
+        <v>341946769.52</v>
       </c>
       <c r="D210" t="n">
-        <v>138355650385.4038</v>
+        <v>138394578985.5095</v>
       </c>
       <c r="E210" t="n">
-        <v>404.62523194839</v>
+        <v>404.7255050245911</v>
       </c>
       <c r="F210" t="n">
-        <v>-0.3246410501956755</v>
+        <v>-0.3244736846581617</v>
       </c>
       <c r="G210" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="H210" t="n">
         <v>2</v>
       </c>
       <c r="I210" t="n">
-        <v>892.0367863534209</v>
+        <v>892.2578483772135</v>
       </c>
     </row>
     <row r="211" spans="1:9">
@@ -9853,25 +9973,25 @@
         <v>6</v>
       </c>
       <c r="C211" t="n">
-        <v>374914808.49</v>
+        <v>374930071.58</v>
       </c>
       <c r="D211" t="n">
-        <v>160778362604.1436</v>
+        <v>160818930718.2976</v>
       </c>
       <c r="E211" t="n">
-        <v>428.8397229538402</v>
+        <v>428.930467061731</v>
       </c>
       <c r="F211" t="n">
-        <v>-0.2842247045892974</v>
+        <v>-0.2840732438286549</v>
       </c>
       <c r="G211" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="H211" t="n">
         <v>2</v>
       </c>
       <c r="I211" t="n">
-        <v>945.4200532240362</v>
+        <v>945.6201076842923</v>
       </c>
     </row>
     <row r="212" spans="1:9">
@@ -9882,25 +10002,25 @@
         <v>7</v>
       </c>
       <c r="C212" t="n">
-        <v>414393752.72</v>
+        <v>414418886.95</v>
       </c>
       <c r="D212" t="n">
-        <v>190379962916.0775</v>
+        <v>190424421326.2244</v>
       </c>
       <c r="E212" t="n">
-        <v>459.4180333715469</v>
+        <v>459.4974488920897</v>
       </c>
       <c r="F212" t="n">
-        <v>-0.2331865241202971</v>
+        <v>-0.2330539718761039</v>
       </c>
       <c r="G212" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="H212" t="n">
         <v>3</v>
       </c>
       <c r="I212" t="n">
-        <v>1012.832996370912</v>
+        <v>1013.008075827501</v>
       </c>
     </row>
     <row r="213" spans="1:9">
@@ -9911,25 +10031,25 @@
         <v>8</v>
       </c>
       <c r="C213" t="n">
-        <v>411007209.6</v>
+        <v>411030574.1700001</v>
       </c>
       <c r="D213" t="n">
-        <v>187650671331.7682</v>
+        <v>187694470242.0007</v>
       </c>
       <c r="E213" t="n">
-        <v>456.5629676287027</v>
+        <v>456.6435735857723</v>
       </c>
       <c r="F213" t="n">
-        <v>-0.2379519071203259</v>
+        <v>-0.237817367921541</v>
       </c>
       <c r="G213" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="H213" t="n">
         <v>3</v>
       </c>
       <c r="I213" t="n">
-        <v>1006.538718434238</v>
+        <v>1006.716422327194</v>
       </c>
     </row>
     <row r="214" spans="1:9">
@@ -9940,25 +10060,25 @@
         <v>9</v>
       </c>
       <c r="C214" t="n">
-        <v>358900117.72</v>
+        <v>358919294.5599999</v>
       </c>
       <c r="D214" t="n">
-        <v>160400518582.8232</v>
+        <v>160439677991.4717</v>
       </c>
       <c r="E214" t="n">
-        <v>446.9224462834014</v>
+        <v>447.0076711483429</v>
       </c>
       <c r="F214" t="n">
-        <v>-0.2540428768801142</v>
+        <v>-0.2539006282738991</v>
       </c>
       <c r="G214" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="H214" t="n">
         <v>3</v>
       </c>
       <c r="I214" t="n">
-        <v>985.2852250763867</v>
+        <v>985.4731118136368</v>
       </c>
     </row>
     <row r="215" spans="1:9">
@@ -9969,25 +10089,25 @@
         <v>10</v>
       </c>
       <c r="C215" t="n">
-        <v>327270536.35</v>
+        <v>327291940.5099999</v>
       </c>
       <c r="D215" t="n">
-        <v>140826059524.6895</v>
+        <v>140855078589.95</v>
       </c>
       <c r="E215" t="n">
-        <v>430.3047292166955</v>
+        <v>430.3652524118492</v>
       </c>
       <c r="F215" t="n">
-        <v>-0.281779466346555</v>
+        <v>-0.2816784472348181</v>
       </c>
       <c r="G215" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="H215" t="n">
         <v>4</v>
       </c>
       <c r="I215" t="n">
-        <v>948.6498060311267</v>
+        <v>948.7832354671627</v>
       </c>
     </row>
     <row r="216" spans="1:9">
@@ -9998,25 +10118,25 @@
         <v>11</v>
       </c>
       <c r="C216" t="n">
-        <v>324213677.9899999</v>
+        <v>324233265.98</v>
       </c>
       <c r="D216" t="n">
-        <v>138104333263.7313</v>
+        <v>138148501905.7901</v>
       </c>
       <c r="E216" t="n">
-        <v>425.967016937487</v>
+        <v>426.0775077727886</v>
       </c>
       <c r="F216" t="n">
-        <v>-0.2890195309251605</v>
+        <v>-0.2888351109518114</v>
       </c>
       <c r="G216" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="H216" t="n">
         <v>4</v>
       </c>
       <c r="I216" t="n">
-        <v>939.0868855403841</v>
+        <v>939.33047363589</v>
       </c>
     </row>
     <row r="217" spans="1:9">
@@ -10027,25 +10147,25 @@
         <v>12</v>
       </c>
       <c r="C217" t="n">
-        <v>340219127.72</v>
+        <v>343900260.12</v>
       </c>
       <c r="D217" t="n">
-        <v>145846975412.7629</v>
+        <v>145876422922.895</v>
       </c>
       <c r="E217" t="n">
-        <v>428.6854075200465</v>
+        <v>424.1823570357088</v>
       </c>
       <c r="F217" t="n">
-        <v>-0.2844822720889901</v>
+        <v>-0.2919983022470057</v>
       </c>
       <c r="G217" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="H217" t="n">
         <v>4</v>
       </c>
       <c r="I217" t="n">
-        <v>945.0798494186946</v>
+        <v>935.1524243209236</v>
       </c>
     </row>
     <row r="218" spans="1:9">
@@ -10056,25 +10176,25 @@
         <v>1</v>
       </c>
       <c r="C218" t="n">
-        <v>359574970.19</v>
+        <v>361338960.48</v>
       </c>
       <c r="D218" t="n">
-        <v>151447205697.6722</v>
+        <v>151697682097.0909</v>
       </c>
       <c r="E218" t="n">
-        <v>421.183948420123</v>
+        <v>419.8209954873863</v>
       </c>
       <c r="F218" t="n">
-        <v>-0.2970029384728666</v>
+        <v>-0.2992778397607903</v>
       </c>
       <c r="G218" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="H218" t="n">
         <v>1</v>
       </c>
       <c r="I218" t="n">
-        <v>928.5421326870031</v>
+        <v>925.5373666514917</v>
       </c>
     </row>
     <row r="219" spans="1:9">
@@ -10085,25 +10205,25 @@
         <v>2</v>
       </c>
       <c r="C219" t="n">
-        <v>315655291.46</v>
+        <v>316990404.61</v>
       </c>
       <c r="D219" t="n">
-        <v>126454918973.7381</v>
+        <v>126194390756.1519</v>
       </c>
       <c r="E219" t="n">
-        <v>400.6108004362806</v>
+        <v>398.1016110295562</v>
       </c>
       <c r="F219" t="n">
-        <v>-0.3313415276647265</v>
+        <v>-0.3355296093481782</v>
       </c>
       <c r="G219" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="H219" t="n">
         <v>1</v>
       </c>
       <c r="I219" t="n">
-        <v>883.1865706418242</v>
+        <v>877.6548116757598</v>
       </c>
     </row>
     <row r="220" spans="1:9">
@@ -10114,25 +10234,25 @@
         <v>3</v>
       </c>
       <c r="C220" t="n">
-        <v>326548929.91</v>
+        <v>329458732.27</v>
       </c>
       <c r="D220" t="n">
-        <v>126528091642.5943</v>
+        <v>127270056508.8244</v>
       </c>
       <c r="E220" t="n">
-        <v>387.4705443912087</v>
+        <v>386.3004499286524</v>
       </c>
       <c r="F220" t="n">
-        <v>-0.3532738957477223</v>
+        <v>-0.3552268974515427</v>
       </c>
       <c r="G220" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="H220" t="n">
         <v>1</v>
       </c>
       <c r="I220" t="n">
-        <v>854.2175621648587</v>
+        <v>851.6379719127069</v>
       </c>
     </row>
     <row r="221" spans="1:9">
@@ -10143,25 +10263,25 @@
         <v>4</v>
       </c>
       <c r="C221" t="n">
-        <v>297333946.63</v>
+        <v>299823167.99</v>
       </c>
       <c r="D221" t="n">
-        <v>103841083288.9281</v>
+        <v>104725567160.1998</v>
       </c>
       <c r="E221" t="n">
-        <v>349.2405911463152</v>
+        <v>349.2911100308721</v>
       </c>
       <c r="F221" t="n">
-        <v>-0.4170834138793867</v>
+        <v>-0.4169990929371277</v>
       </c>
       <c r="G221" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="H221" t="n">
         <v>2</v>
       </c>
       <c r="I221" t="n">
-        <v>769.9358072411666</v>
+        <v>770.0471811740608</v>
       </c>
     </row>
     <row r="222" spans="1:9">
@@ -10172,25 +10292,25 @@
         <v>5</v>
       </c>
       <c r="C222" t="n">
-        <v>331679522.33</v>
+        <v>333868759.6700001</v>
       </c>
       <c r="D222" t="n">
-        <v>123189946951.3786</v>
+        <v>124336029296.85</v>
       </c>
       <c r="E222" t="n">
-        <v>371.4125794863283</v>
+        <v>372.409893695191</v>
       </c>
       <c r="F222" t="n">
-        <v>-0.3800762042986087</v>
+        <v>-0.3784115896786081</v>
       </c>
       <c r="G222" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="H222" t="n">
         <v>2</v>
       </c>
       <c r="I222" t="n">
-        <v>818.8161727355596</v>
+        <v>821.0148516404181</v>
       </c>
     </row>
     <row r="223" spans="1:9">
@@ -10201,25 +10321,25 @@
         <v>6</v>
       </c>
       <c r="C223" t="n">
-        <v>354890953.5800002</v>
+        <v>356505690.02</v>
       </c>
       <c r="D223" t="n">
-        <v>139120102636.1018</v>
+        <v>139790363041.5156</v>
       </c>
       <c r="E223" t="n">
-        <v>392.008027346747</v>
+        <v>392.1125719863639</v>
       </c>
       <c r="F223" t="n">
-        <v>-0.3457003944392367</v>
+        <v>-0.3455258992460444</v>
       </c>
       <c r="G223" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="H223" t="n">
         <v>2</v>
       </c>
       <c r="I223" t="n">
-        <v>864.2208970886386</v>
+        <v>864.4513762011378</v>
       </c>
     </row>
     <row r="224" spans="1:9">
@@ -10230,25 +10350,25 @@
         <v>7</v>
       </c>
       <c r="C224" t="n">
-        <v>415190456.2900001</v>
+        <v>413677113.4200001</v>
       </c>
       <c r="D224" t="n">
-        <v>177588375177.8423</v>
+        <v>178868344373.9786</v>
       </c>
       <c r="E224" t="n">
-        <v>427.7274982780464</v>
+        <v>432.3863674623361</v>
       </c>
       <c r="F224" t="n">
-        <v>-0.2860811159786059</v>
+        <v>-0.2783050092231603</v>
       </c>
       <c r="G224" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="H224" t="n">
         <v>3</v>
       </c>
       <c r="I224" t="n">
-        <v>942.9680427037813</v>
+        <v>953.238985707466</v>
       </c>
     </row>
     <row r="225" spans="1:9">
@@ -10259,25 +10379,25 @@
         <v>8</v>
       </c>
       <c r="C225" t="n">
-        <v>405103765.2099999</v>
+        <v>404953556.2000001</v>
       </c>
       <c r="D225" t="n">
-        <v>171782632561.9474</v>
+        <v>173131780597.812</v>
       </c>
       <c r="E225" t="n">
-        <v>424.0460033070732</v>
+        <v>427.5349060332861</v>
       </c>
       <c r="F225" t="n">
-        <v>-0.2922258899101127</v>
+        <v>-0.2864025712065348</v>
       </c>
       <c r="G225" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="H225" t="n">
         <v>3</v>
       </c>
       <c r="I225" t="n">
-        <v>934.8518188907736</v>
+        <v>942.5434538409824</v>
       </c>
     </row>
     <row r="226" spans="1:9">
@@ -10288,25 +10408,25 @@
         <v>9</v>
       </c>
       <c r="C226" t="n">
-        <v>362633351.4</v>
+        <v>363607055.42</v>
       </c>
       <c r="D226" t="n">
-        <v>152167046728.8568</v>
+        <v>152677718202.1345</v>
       </c>
       <c r="E226" t="n">
-        <v>419.6168006648954</v>
+        <v>419.89756778998</v>
       </c>
       <c r="F226" t="n">
-        <v>-0.2996186608218221</v>
+        <v>-0.2991500331244745</v>
       </c>
       <c r="G226" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="H226" t="n">
         <v>3</v>
       </c>
       <c r="I226" t="n">
-        <v>925.0871987458283</v>
+        <v>925.70617794979</v>
       </c>
     </row>
     <row r="227" spans="1:9">
@@ -10317,25 +10437,25 @@
         <v>10</v>
       </c>
       <c r="C227" t="n">
-        <v>324571214.7</v>
+        <v>323034833.3100001</v>
       </c>
       <c r="D227" t="n">
-        <v>124662728045.8329</v>
+        <v>124378724851.0999</v>
       </c>
       <c r="E227" t="n">
-        <v>384.0843623827152</v>
+        <v>385.0319285280917</v>
       </c>
       <c r="F227" t="n">
-        <v>-0.3589257635615272</v>
+        <v>-0.357344183308289</v>
       </c>
       <c r="G227" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="H227" t="n">
         <v>4</v>
       </c>
       <c r="I227" t="n">
-        <v>846.752385308934</v>
+        <v>848.8413896330306</v>
       </c>
     </row>
     <row r="228" spans="1:9">
@@ -10346,25 +10466,25 @@
         <v>11</v>
       </c>
       <c r="C228" t="n">
-        <v>318668785.02</v>
+        <v>317893099.79</v>
       </c>
       <c r="D228" t="n">
-        <v>124778566256.1873</v>
+        <v>125228939378.1823</v>
       </c>
       <c r="E228" t="n">
-        <v>391.5619355323934</v>
+        <v>393.9341227000789</v>
       </c>
       <c r="F228" t="n">
-        <v>-0.3464449651567066</v>
+        <v>-0.3424855535634331</v>
       </c>
       <c r="G228" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="H228" t="n">
         <v>4</v>
       </c>
       <c r="I228" t="n">
-        <v>863.2374430747142</v>
+        <v>868.4671669045941</v>
       </c>
     </row>
     <row r="229" spans="1:9">
@@ -10375,25 +10495,344 @@
         <v>12</v>
       </c>
       <c r="C229" t="n">
-        <v>339113052.3699999</v>
+        <v>340256890.15</v>
       </c>
       <c r="D229" t="n">
-        <v>126713811428.1058</v>
+        <v>127420498637.0739</v>
       </c>
       <c r="E229" t="n">
-        <v>373.6624424879133</v>
+        <v>374.4832281894467</v>
       </c>
       <c r="F229" t="n">
-        <v>-0.3763209636611493</v>
+        <v>-0.3749509923256181</v>
       </c>
       <c r="G229" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="H229" t="n">
         <v>4</v>
       </c>
       <c r="I229" t="n">
-        <v>823.7762207088538</v>
+        <v>825.585724866454</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9">
+      <c r="A230" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B230" t="n">
+        <v>1</v>
+      </c>
+      <c r="C230" t="n">
+        <v>342607271.51</v>
+      </c>
+      <c r="D230" t="n">
+        <v>122256497598.3264</v>
+      </c>
+      <c r="E230" t="n">
+        <v>356.8415143656925</v>
+      </c>
+      <c r="F230" t="n">
+        <v>-0.404396732185654</v>
+      </c>
+      <c r="G230" t="s">
+        <v>317</v>
+      </c>
+      <c r="H230" t="n">
+        <v>1</v>
+      </c>
+      <c r="I230" t="n">
+        <v>786.6928025706057</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9">
+      <c r="A231" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B231" t="n">
+        <v>2</v>
+      </c>
+      <c r="C231" t="n">
+        <v>320228161.8800001</v>
+      </c>
+      <c r="D231" t="n">
+        <v>110058566328.8358</v>
+      </c>
+      <c r="E231" t="n">
+        <v>343.6879682370922</v>
+      </c>
+      <c r="F231" t="n">
+        <v>-0.4263512827134061</v>
+      </c>
+      <c r="G231" t="s">
+        <v>318</v>
+      </c>
+      <c r="H231" t="n">
+        <v>1</v>
+      </c>
+      <c r="I231" t="n">
+        <v>757.6944947754934</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9">
+      <c r="A232" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B232" t="n">
+        <v>3</v>
+      </c>
+      <c r="C232" t="n">
+        <v>310249786.54</v>
+      </c>
+      <c r="D232" t="n">
+        <v>104329887876.093</v>
+      </c>
+      <c r="E232" t="n">
+        <v>336.2770657785512</v>
+      </c>
+      <c r="F232" t="n">
+        <v>-0.4387208012365141</v>
+      </c>
+      <c r="G232" t="s">
+        <v>319</v>
+      </c>
+      <c r="H232" t="n">
+        <v>1</v>
+      </c>
+      <c r="I232" t="n">
+        <v>741.3564192153937</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9">
+      <c r="A233" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B233" t="n">
+        <v>4</v>
+      </c>
+      <c r="C233" t="n">
+        <v>279442889.37</v>
+      </c>
+      <c r="D233" t="n">
+        <v>87266469145.20724</v>
+      </c>
+      <c r="E233" t="n">
+        <v>312.2873133109533</v>
+      </c>
+      <c r="F233" t="n">
+        <v>-0.4787620363185841</v>
+      </c>
+      <c r="G233" t="s">
+        <v>320</v>
+      </c>
+      <c r="H233" t="n">
+        <v>2</v>
+      </c>
+      <c r="I233" t="n">
+        <v>688.4686109253278</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9">
+      <c r="A234" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B234" t="n">
+        <v>5</v>
+      </c>
+      <c r="C234" t="n">
+        <v>308108815.53</v>
+      </c>
+      <c r="D234" t="n">
+        <v>97697493019.18562</v>
+      </c>
+      <c r="E234" t="n">
+        <v>317.0876264969219</v>
+      </c>
+      <c r="F234" t="n">
+        <v>-0.4707498457381877</v>
+      </c>
+      <c r="G234" t="s">
+        <v>321</v>
+      </c>
+      <c r="H234" t="n">
+        <v>2</v>
+      </c>
+      <c r="I234" t="n">
+        <v>699.051381375114</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9">
+      <c r="A235" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B235" t="n">
+        <v>6</v>
+      </c>
+      <c r="C235" t="n">
+        <v>356992814.96</v>
+      </c>
+      <c r="D235" t="n">
+        <v>129195411036.1445</v>
+      </c>
+      <c r="E235" t="n">
+        <v>361.8991913061905</v>
+      </c>
+      <c r="F235" t="n">
+        <v>-0.3959549764144273</v>
+      </c>
+      <c r="G235" t="s">
+        <v>322</v>
+      </c>
+      <c r="H235" t="n">
+        <v>2</v>
+      </c>
+      <c r="I235" t="n">
+        <v>797.8429571536275</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9">
+      <c r="A236" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B236" t="n">
+        <v>7</v>
+      </c>
+      <c r="C236" t="n">
+        <v>418811407.12</v>
+      </c>
+      <c r="D236" t="n">
+        <v>172744859346.393</v>
+      </c>
+      <c r="E236" t="n">
+        <v>412.4645518475511</v>
+      </c>
+      <c r="F236" t="n">
+        <v>-0.3115564612075306</v>
+      </c>
+      <c r="G236" t="s">
+        <v>323</v>
+      </c>
+      <c r="H236" t="n">
+        <v>3</v>
+      </c>
+      <c r="I236" t="n">
+        <v>909.3193510031113</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9">
+      <c r="A237" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B237" t="n">
+        <v>8</v>
+      </c>
+      <c r="C237" t="n">
+        <v>403692201.02</v>
+      </c>
+      <c r="D237" t="n">
+        <v>168389271706.7094</v>
+      </c>
+      <c r="E237" t="n">
+        <v>417.122925043496</v>
+      </c>
+      <c r="F237" t="n">
+        <v>-0.303781182304975</v>
+      </c>
+      <c r="G237" t="s">
+        <v>324</v>
+      </c>
+      <c r="H237" t="n">
+        <v>3</v>
+      </c>
+      <c r="I237" t="n">
+        <v>919.5892005508913</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9">
+      <c r="A238" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B238" t="n">
+        <v>9</v>
+      </c>
+      <c r="C238" t="n">
+        <v>337662516.7600001</v>
+      </c>
+      <c r="D238" t="n">
+        <v>131273617211.3669</v>
+      </c>
+      <c r="E238" t="n">
+        <v>388.7716601504577</v>
+      </c>
+      <c r="F238" t="n">
+        <v>-0.3511022067294449</v>
+      </c>
+      <c r="G238" t="s">
+        <v>325</v>
+      </c>
+      <c r="H238" t="n">
+        <v>3</v>
+      </c>
+      <c r="I238" t="n">
+        <v>857.0860019676991</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9">
+      <c r="A239" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B239" t="n">
+        <v>10</v>
+      </c>
+      <c r="C239" t="n">
+        <v>317474008.16</v>
+      </c>
+      <c r="D239" t="n">
+        <v>117065420659.7417</v>
+      </c>
+      <c r="E239" t="n">
+        <v>368.740172898637</v>
+      </c>
+      <c r="F239" t="n">
+        <v>-0.3845367113654135</v>
+      </c>
+      <c r="G239" t="s">
+        <v>326</v>
+      </c>
+      <c r="H239" t="n">
+        <v>4</v>
+      </c>
+      <c r="I239" t="n">
+        <v>812.9245851723352</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9">
+      <c r="A240" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B240" t="n">
+        <v>11</v>
+      </c>
+      <c r="C240" t="n">
+        <v>304229876.47</v>
+      </c>
+      <c r="D240" t="n">
+        <v>107746956147.4566</v>
+      </c>
+      <c r="E240" t="n">
+        <v>354.1629684686195</v>
+      </c>
+      <c r="F240" t="n">
+        <v>-0.4088674863581983</v>
+      </c>
+      <c r="G240" t="s">
+        <v>327</v>
+      </c>
+      <c r="H240" t="n">
+        <v>4</v>
+      </c>
+      <c r="I240" t="n">
+        <v>780.7876802859184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2020 quarter 2 update. no changes made to the code
</commit_message>
<xml_diff>
--- a/web_files/US Power Sector CO2 Emissions Intensity.xlsx
+++ b/web_files/US Power Sector CO2 Emissions Intensity.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="338">
   <si>
     <t>year</t>
   </si>
@@ -286,6 +286,9 @@
     <t>2021 Q1</t>
   </si>
   <si>
+    <t>2021 Q2</t>
+  </si>
+  <si>
     <t>month</t>
   </si>
   <si>
@@ -1019,6 +1022,15 @@
   </si>
   <si>
     <t>2021-03-01</t>
+  </si>
+  <si>
+    <t>2021-04-01</t>
+  </si>
+  <si>
+    <t>2021-05-01</t>
+  </si>
+  <si>
+    <t>2021-06-01</t>
   </si>
 </sst>
 </file>
@@ -1723,16 +1735,16 @@
         <v>4058030988.1</v>
       </c>
       <c r="C18" t="n">
-        <v>1780378551348.644</v>
+        <v>1780378551379.489</v>
       </c>
       <c r="D18" t="n">
-        <v>438.7296589329967</v>
+        <v>438.7296589405975</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.2677174374958625</v>
+        <v>-0.2677174374831761</v>
       </c>
       <c r="F18" t="n">
-        <v>967.2234060836847</v>
+        <v>967.2234061004413</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1743,16 +1755,16 @@
         <v>4207602186.04</v>
       </c>
       <c r="C19" t="n">
-        <v>1798487721116.658</v>
+        <v>1798504282118.086</v>
       </c>
       <c r="D19" t="n">
-        <v>427.4376810345065</v>
+        <v>427.4416170058024</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.2865648492057448</v>
+        <v>-0.2865582796860241</v>
       </c>
       <c r="F19" t="n">
-        <v>942.3291116086732</v>
+        <v>942.337788850992</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1763,16 +1775,16 @@
         <v>4162381332.79</v>
       </c>
       <c r="C20" t="n">
-        <v>1655767794801.074</v>
+        <v>1655808982664.746</v>
       </c>
       <c r="D20" t="n">
-        <v>397.7933933533261</v>
+        <v>397.80328861769</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.3360440546909159</v>
+        <v>-0.3360275385302288</v>
       </c>
       <c r="F20" t="n">
-        <v>876.9753149867425</v>
+        <v>876.9971300865594</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1783,16 +1795,16 @@
         <v>4048092156.28</v>
       </c>
       <c r="C21" t="n">
-        <v>1481509583377.116</v>
+        <v>1481612130449.878</v>
       </c>
       <c r="D21" t="n">
-        <v>365.9772372224232</v>
+        <v>366.0025694206051</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.3891483203045779</v>
+        <v>-0.3891060383967542</v>
       </c>
       <c r="F21" t="n">
-        <v>806.8334171805542</v>
+        <v>806.8892645446663</v>
       </c>
     </row>
   </sheetData>
@@ -1806,7 +1818,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3593,19 +3605,19 @@
         <v>982079072.27</v>
       </c>
       <c r="D69" t="n">
-        <v>424056131667.5315</v>
+        <v>424056131698.3757</v>
       </c>
       <c r="E69" t="n">
-        <v>431.794285858631</v>
+        <v>431.7942858900381</v>
       </c>
       <c r="F69" t="n">
-        <v>-0.2792932511282715</v>
+        <v>-0.27929325107585</v>
       </c>
       <c r="G69" t="s">
         <v>75</v>
       </c>
       <c r="H69" t="n">
-        <v>951.933682603938</v>
+        <v>951.9336826731779</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3619,19 +3631,19 @@
         <v>1007451607.32</v>
       </c>
       <c r="D70" t="n">
-        <v>419654663331.7893</v>
+        <v>419654783951.9741</v>
       </c>
       <c r="E70" t="n">
-        <v>416.5506911524466</v>
+        <v>416.5508108804654</v>
       </c>
       <c r="F70" t="n">
-        <v>-0.3047362964431631</v>
+        <v>-0.3047360966054303</v>
       </c>
       <c r="G70" t="s">
         <v>76</v>
       </c>
       <c r="H70" t="n">
-        <v>918.3276537146839</v>
+        <v>918.327917667074</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -3645,19 +3657,19 @@
         <v>1020356356.43</v>
       </c>
       <c r="D71" t="n">
-        <v>415364914487.4792</v>
+        <v>415367899286.621</v>
       </c>
       <c r="E71" t="n">
-        <v>407.0782838465854</v>
+        <v>407.0812090982614</v>
       </c>
       <c r="F71" t="n">
-        <v>-0.3205466674855237</v>
+        <v>-0.3205417849553603</v>
       </c>
       <c r="G71" t="s">
         <v>77</v>
       </c>
       <c r="H71" t="n">
-        <v>897.4447845681821</v>
+        <v>897.4512335780272</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -3671,19 +3683,19 @@
         <v>1184368755.68</v>
       </c>
       <c r="D72" t="n">
-        <v>538574941633.8301</v>
+        <v>538581837048.5731</v>
       </c>
       <c r="E72" t="n">
-        <v>454.7358574353895</v>
+        <v>454.7416794521472</v>
       </c>
       <c r="F72" t="n">
-        <v>-0.2410015321162536</v>
+        <v>-0.2409918146028292</v>
       </c>
       <c r="G72" t="s">
         <v>78</v>
       </c>
       <c r="H72" t="n">
-        <v>1002.51067130206</v>
+        <v>1002.523506520204</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3697,19 +3709,19 @@
         <v>995425466.61</v>
       </c>
       <c r="D73" t="n">
-        <v>424893201663.5593</v>
+        <v>424899761830.9181</v>
       </c>
       <c r="E73" t="n">
-        <v>426.8458221292717</v>
+        <v>426.8524124442463</v>
       </c>
       <c r="F73" t="n">
-        <v>-0.2875527194054034</v>
+        <v>-0.2875417195273712</v>
       </c>
       <c r="G73" t="s">
         <v>79</v>
       </c>
       <c r="H73" t="n">
-        <v>941.0242994661924</v>
+        <v>941.0388284745856</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3723,19 +3735,19 @@
         <v>1008004393.08</v>
       </c>
       <c r="D74" t="n">
-        <v>405175112121.652</v>
+        <v>405183038503.726</v>
       </c>
       <c r="E74" t="n">
-        <v>401.9576848108989</v>
+        <v>401.965548250908</v>
       </c>
       <c r="F74" t="n">
-        <v>-0.3290934463664595</v>
+        <v>-0.329080321518657</v>
       </c>
       <c r="G74" t="s">
         <v>80</v>
       </c>
       <c r="H74" t="n">
-        <v>886.1559119341078</v>
+        <v>886.1732476739518</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -3749,19 +3761,19 @@
         <v>990398214.4000002</v>
       </c>
       <c r="D75" t="n">
-        <v>368862866512.5936</v>
+        <v>368873497056.2224</v>
       </c>
       <c r="E75" t="n">
-        <v>372.4389454155639</v>
+        <v>372.4496790209706</v>
       </c>
       <c r="F75" t="n">
-        <v>-0.3783630995257162</v>
+        <v>-0.3783451840921183</v>
       </c>
       <c r="G75" t="s">
         <v>81</v>
       </c>
       <c r="H75" t="n">
-        <v>821.0788990631523</v>
+        <v>821.1025623696316</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -3775,19 +3787,19 @@
         <v>1182402315.25</v>
       </c>
       <c r="D76" t="n">
-        <v>504690217499.8117</v>
+        <v>504700664192.4819</v>
       </c>
       <c r="E76" t="n">
-        <v>426.8345985038966</v>
+        <v>426.8434336461621</v>
       </c>
       <c r="F76" t="n">
-        <v>-0.2875714527300895</v>
+        <v>-0.287556706016512</v>
       </c>
       <c r="G76" t="s">
         <v>82</v>
       </c>
       <c r="H76" t="n">
-        <v>940.9995558616906</v>
+        <v>941.0190338163291</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3801,19 +3813,19 @@
         <v>981576410.0599999</v>
       </c>
       <c r="D77" t="n">
-        <v>377039598667.0168</v>
+        <v>377051782912.3154</v>
       </c>
       <c r="E77" t="n">
-        <v>384.1164017419385</v>
+        <v>384.1288146780827</v>
       </c>
       <c r="F77" t="n">
-        <v>-0.3588722867481973</v>
+        <v>-0.3588515683479188</v>
       </c>
       <c r="G77" t="s">
         <v>83</v>
       </c>
       <c r="H77" t="n">
-        <v>846.8230192802777</v>
+        <v>846.8503848393011</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -3827,19 +3839,19 @@
         <v>974253921.76</v>
       </c>
       <c r="D78" t="n">
-        <v>336699845242.4945</v>
+        <v>336712685568.3041</v>
       </c>
       <c r="E78" t="n">
-        <v>345.5976288340135</v>
+        <v>345.610808484126</v>
       </c>
       <c r="F78" t="n">
-        <v>-0.4231638730479009</v>
+        <v>-0.4231418749272797</v>
       </c>
       <c r="G78" t="s">
         <v>84</v>
       </c>
       <c r="H78" t="n">
-        <v>761.9045325274662</v>
+        <v>761.9335883841043</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3853,19 +3865,19 @@
         <v>944857554.5700001</v>
       </c>
       <c r="D79" t="n">
-        <v>315008309721.3477</v>
+        <v>315020376970.6643</v>
       </c>
       <c r="E79" t="n">
-        <v>333.3923808914312</v>
+        <v>333.4051523925514</v>
       </c>
       <c r="F79" t="n">
-        <v>-0.4435356214752337</v>
+        <v>-0.4435143045950618</v>
       </c>
       <c r="G79" t="s">
         <v>85</v>
       </c>
       <c r="H79" t="n">
-        <v>734.9968429132492</v>
+        <v>735.0249989646188</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3879,19 +3891,19 @@
         <v>1159510253.94</v>
       </c>
       <c r="D80" t="n">
-        <v>472252639915.4503</v>
+        <v>472285435923.179</v>
       </c>
       <c r="E80" t="n">
-        <v>407.2862989445263</v>
+        <v>407.3145833064949</v>
       </c>
       <c r="F80" t="n">
-        <v>-0.3201994700124143</v>
+        <v>-0.3201522606554916</v>
       </c>
       <c r="G80" t="s">
         <v>86</v>
       </c>
       <c r="H80" t="n">
-        <v>897.9033746531027</v>
+        <v>897.9657303574985</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -3905,19 +3917,19 @@
         <v>969470426.01</v>
       </c>
       <c r="D81" t="n">
-        <v>357548788497.8237</v>
+        <v>357593631987.7302</v>
       </c>
       <c r="E81" t="n">
-        <v>368.8083503169551</v>
+        <v>368.8546059723143</v>
       </c>
       <c r="F81" t="n">
-        <v>-0.3844229166091797</v>
+        <v>-0.3843457114119765</v>
       </c>
       <c r="G81" t="s">
         <v>87</v>
       </c>
       <c r="H81" t="n">
-        <v>813.0748891087592</v>
+        <v>813.1768643265642</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -3931,19 +3943,45 @@
         <v>997418941.59</v>
       </c>
       <c r="D82" t="n">
-        <v>377541698471.6443</v>
+        <v>377541945964.0786</v>
       </c>
       <c r="E82" t="n">
-        <v>378.518677286998</v>
+        <v>378.5189254198778</v>
       </c>
       <c r="F82" t="n">
-        <v>-0.3682154344579398</v>
+        <v>-0.3682150202999787</v>
       </c>
       <c r="G82" t="s">
         <v>88</v>
       </c>
       <c r="H82" t="n">
-        <v>834.4822759469157</v>
+        <v>834.4828229806625</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B83" t="n">
+        <v>2</v>
+      </c>
+      <c r="C83" t="n">
+        <v>998141284.0599999</v>
+      </c>
+      <c r="D83" t="n">
+        <v>365530956115.6558</v>
+      </c>
+      <c r="E83" t="n">
+        <v>366.2116395274591</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-0.3887570800109402</v>
+      </c>
+      <c r="G83" t="s">
+        <v>89</v>
+      </c>
+      <c r="H83" t="n">
+        <v>807.3501805022362</v>
       </c>
     </row>
   </sheetData>
@@ -3957,7 +3995,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I244"/>
+  <dimension ref="A1:I247"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3970,7 +4008,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -3985,7 +4023,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -4014,7 +4052,7 @@
         <v>0.07726515958654644</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
@@ -4043,7 +4081,7 @@
         <v>0.06148124887439917</v>
       </c>
       <c r="G3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
@@ -4072,7 +4110,7 @@
         <v>0.04746077038960551</v>
       </c>
       <c r="G4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -4101,7 +4139,7 @@
         <v>0.04727244615802906</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H5" t="n">
         <v>2</v>
@@ -4130,7 +4168,7 @@
         <v>0.04871093696407162</v>
       </c>
       <c r="G6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H6" t="n">
         <v>2</v>
@@ -4159,7 +4197,7 @@
         <v>0.04304157536165719</v>
       </c>
       <c r="G7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H7" t="n">
         <v>2</v>
@@ -4188,7 +4226,7 @@
         <v>0.07078023556064666</v>
       </c>
       <c r="G8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H8" t="n">
         <v>3</v>
@@ -4217,7 +4255,7 @@
         <v>0.07532787659744344</v>
       </c>
       <c r="G9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H9" t="n">
         <v>3</v>
@@ -4246,7 +4284,7 @@
         <v>0.05259835799380738</v>
       </c>
       <c r="G10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H10" t="n">
         <v>3</v>
@@ -4275,7 +4313,7 @@
         <v>0.03553213710629145</v>
       </c>
       <c r="G11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H11" t="n">
         <v>4</v>
@@ -4304,7 +4342,7 @@
         <v>0.02646669802403197</v>
       </c>
       <c r="G12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H12" t="n">
         <v>4</v>
@@ -4333,7 +4371,7 @@
         <v>0.01912175729454257</v>
       </c>
       <c r="G13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H13" t="n">
         <v>4</v>
@@ -4362,7 +4400,7 @@
         <v>0.01111774538231211</v>
       </c>
       <c r="G14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H14" t="n">
         <v>1</v>
@@ -4391,7 +4429,7 @@
         <v>0.005018273091192093</v>
       </c>
       <c r="G15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H15" t="n">
         <v>1</v>
@@ -4420,7 +4458,7 @@
         <v>0.01544195713902331</v>
       </c>
       <c r="G16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H16" t="n">
         <v>1</v>
@@ -4449,7 +4487,7 @@
         <v>0.003355439027818183</v>
       </c>
       <c r="G17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H17" t="n">
         <v>2</v>
@@ -4478,7 +4516,7 @@
         <v>0.00536957613039397</v>
       </c>
       <c r="G18" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H18" t="n">
         <v>2</v>
@@ -4507,7 +4545,7 @@
         <v>0.0145689414097139</v>
       </c>
       <c r="G19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H19" t="n">
         <v>2</v>
@@ -4536,7 +4574,7 @@
         <v>0.03912865348530959</v>
       </c>
       <c r="G20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H20" t="n">
         <v>3</v>
@@ -4565,7 +4603,7 @@
         <v>0.04573043199637251</v>
       </c>
       <c r="G21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H21" t="n">
         <v>3</v>
@@ -4594,7 +4632,7 @@
         <v>0.05004182162970362</v>
       </c>
       <c r="G22" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H22" t="n">
         <v>3</v>
@@ -4623,7 +4661,7 @@
         <v>0.0547357353567896</v>
       </c>
       <c r="G23" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H23" t="n">
         <v>4</v>
@@ -4652,7 +4690,7 @@
         <v>0.03397983951034167</v>
       </c>
       <c r="G24" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H24" t="n">
         <v>4</v>
@@ -4681,7 +4719,7 @@
         <v>0.03489294255166995</v>
       </c>
       <c r="G25" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H25" t="n">
         <v>4</v>
@@ -4710,7 +4748,7 @@
         <v>0.05407231572896915</v>
       </c>
       <c r="G26" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H26" t="n">
         <v>1</v>
@@ -4739,7 +4777,7 @@
         <v>0.0446998960634503</v>
       </c>
       <c r="G27" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H27" t="n">
         <v>1</v>
@@ -4768,7 +4806,7 @@
         <v>0.02564607186253928</v>
       </c>
       <c r="G28" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H28" t="n">
         <v>1</v>
@@ -4797,7 +4835,7 @@
         <v>-0.005255460204990879</v>
       </c>
       <c r="G29" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H29" t="n">
         <v>2</v>
@@ -4826,7 +4864,7 @@
         <v>-0.005159282455205773</v>
       </c>
       <c r="G30" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H30" t="n">
         <v>2</v>
@@ -4855,7 +4893,7 @@
         <v>0.01662217479072057</v>
       </c>
       <c r="G31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H31" t="n">
         <v>2</v>
@@ -4884,7 +4922,7 @@
         <v>0.03768728145702852</v>
       </c>
       <c r="G32" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H32" t="n">
         <v>3</v>
@@ -4913,7 +4951,7 @@
         <v>0.04140058597533856</v>
       </c>
       <c r="G33" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H33" t="n">
         <v>3</v>
@@ -4942,7 +4980,7 @@
         <v>0.04146258828233757</v>
       </c>
       <c r="G34" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H34" t="n">
         <v>3</v>
@@ -4971,7 +5009,7 @@
         <v>0.05070299868862761</v>
       </c>
       <c r="G35" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H35" t="n">
         <v>4</v>
@@ -5000,7 +5038,7 @@
         <v>0.04234991120899041</v>
       </c>
       <c r="G36" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H36" t="n">
         <v>4</v>
@@ -5029,7 +5067,7 @@
         <v>0.03310887154716038</v>
       </c>
       <c r="G37" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H37" t="n">
         <v>4</v>
@@ -5058,7 +5096,7 @@
         <v>0.03014022625659499</v>
       </c>
       <c r="G38" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H38" t="n">
         <v>1</v>
@@ -5087,7 +5125,7 @@
         <v>0.01239560014339367</v>
       </c>
       <c r="G39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H39" t="n">
         <v>1</v>
@@ -5116,7 +5154,7 @@
         <v>-0.01037094285092945</v>
       </c>
       <c r="G40" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H40" t="n">
         <v>1</v>
@@ -5145,7 +5183,7 @@
         <v>-0.02234624922534889</v>
       </c>
       <c r="G41" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H41" t="n">
         <v>2</v>
@@ -5174,7 +5212,7 @@
         <v>-0.01332959283944984</v>
       </c>
       <c r="G42" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H42" t="n">
         <v>2</v>
@@ -5203,7 +5241,7 @@
         <v>-0.007522138257441214</v>
       </c>
       <c r="G43" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H43" t="n">
         <v>2</v>
@@ -5232,7 +5270,7 @@
         <v>0.002774173076043244</v>
       </c>
       <c r="G44" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H44" t="n">
         <v>3</v>
@@ -5261,7 +5299,7 @@
         <v>0.005812723595943646</v>
       </c>
       <c r="G45" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H45" t="n">
         <v>3</v>
@@ -5290,7 +5328,7 @@
         <v>-0.0001281622510707689</v>
       </c>
       <c r="G46" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H46" t="n">
         <v>3</v>
@@ -5319,7 +5357,7 @@
         <v>0.005798551352125575</v>
       </c>
       <c r="G47" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H47" t="n">
         <v>4</v>
@@ -5348,7 +5386,7 @@
         <v>0.0142697616731208</v>
       </c>
       <c r="G48" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H48" t="n">
         <v>4</v>
@@ -5377,7 +5415,7 @@
         <v>0.006630546904983436</v>
       </c>
       <c r="G49" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H49" t="n">
         <v>4</v>
@@ -5406,7 +5444,7 @@
         <v>0.01135874913719794</v>
       </c>
       <c r="G50" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H50" t="n">
         <v>1</v>
@@ -5435,7 +5473,7 @@
         <v>0.00158584139446698</v>
       </c>
       <c r="G51" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H51" t="n">
         <v>1</v>
@@ -5464,7 +5502,7 @@
         <v>0.0004943352228414668</v>
       </c>
       <c r="G52" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H52" t="n">
         <v>1</v>
@@ -5493,7 +5531,7 @@
         <v>-0.03023291224285088</v>
       </c>
       <c r="G53" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H53" t="n">
         <v>2</v>
@@ -5522,7 +5560,7 @@
         <v>-0.03619156271650293</v>
       </c>
       <c r="G54" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H54" t="n">
         <v>2</v>
@@ -5551,7 +5589,7 @@
         <v>-0.007018965988378289</v>
       </c>
       <c r="G55" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H55" t="n">
         <v>2</v>
@@ -5580,7 +5618,7 @@
         <v>-0.0008959033638951873</v>
       </c>
       <c r="G56" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H56" t="n">
         <v>3</v>
@@ -5609,7 +5647,7 @@
         <v>0.007925452227224232</v>
       </c>
       <c r="G57" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H57" t="n">
         <v>3</v>
@@ -5638,7 +5676,7 @@
         <v>0.01721030590351288</v>
       </c>
       <c r="G58" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H58" t="n">
         <v>3</v>
@@ -5667,7 +5705,7 @@
         <v>0.02231843704751483</v>
       </c>
       <c r="G59" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H59" t="n">
         <v>4</v>
@@ -5696,7 +5734,7 @@
         <v>0.002897748801680964</v>
       </c>
       <c r="G60" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H60" t="n">
         <v>4</v>
@@ -5725,7 +5763,7 @@
         <v>0.00389971424966281</v>
       </c>
       <c r="G61" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H61" t="n">
         <v>4</v>
@@ -5754,7 +5792,7 @@
         <v>-0.02748121131636642</v>
       </c>
       <c r="G62" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H62" t="n">
         <v>1</v>
@@ -5783,7 +5821,7 @@
         <v>-0.01857254232013877</v>
       </c>
       <c r="G63" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H63" t="n">
         <v>1</v>
@@ -5812,7 +5850,7 @@
         <v>-0.02435619078134472</v>
       </c>
       <c r="G64" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H64" t="n">
         <v>1</v>
@@ -5841,7 +5879,7 @@
         <v>-0.06369815302300276</v>
       </c>
       <c r="G65" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H65" t="n">
         <v>2</v>
@@ -5870,7 +5908,7 @@
         <v>-0.05404582225952413</v>
       </c>
       <c r="G66" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H66" t="n">
         <v>2</v>
@@ -5899,7 +5937,7 @@
         <v>-0.04243926553323214</v>
       </c>
       <c r="G67" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H67" t="n">
         <v>2</v>
@@ -5928,7 +5966,7 @@
         <v>-0.01354297585931169</v>
       </c>
       <c r="G68" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H68" t="n">
         <v>3</v>
@@ -5957,7 +5995,7 @@
         <v>-0.004118886890496862</v>
       </c>
       <c r="G69" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H69" t="n">
         <v>3</v>
@@ -5986,7 +6024,7 @@
         <v>-0.01455882450582037</v>
       </c>
       <c r="G70" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H70" t="n">
         <v>3</v>
@@ -6015,7 +6053,7 @@
         <v>0.00439522235340898</v>
       </c>
       <c r="G71" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H71" t="n">
         <v>4</v>
@@ -6044,7 +6082,7 @@
         <v>-0.003746313420402704</v>
       </c>
       <c r="G72" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H72" t="n">
         <v>4</v>
@@ -6073,7 +6111,7 @@
         <v>-0.01605853233048685</v>
       </c>
       <c r="G73" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H73" t="n">
         <v>4</v>
@@ -6102,7 +6140,7 @@
         <v>-0.03511432398711213</v>
       </c>
       <c r="G74" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H74" t="n">
         <v>1</v>
@@ -6131,7 +6169,7 @@
         <v>-0.008437620703637254</v>
       </c>
       <c r="G75" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H75" t="n">
         <v>1</v>
@@ -6160,7 +6198,7 @@
         <v>-0.03117857292861368</v>
       </c>
       <c r="G76" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H76" t="n">
         <v>1</v>
@@ -6189,7 +6227,7 @@
         <v>-0.03928361585166878</v>
       </c>
       <c r="G77" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H77" t="n">
         <v>2</v>
@@ -6218,7 +6256,7 @@
         <v>-0.03788195719455209</v>
       </c>
       <c r="G78" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H78" t="n">
         <v>2</v>
@@ -6247,7 +6285,7 @@
         <v>-0.0177532915761511</v>
       </c>
       <c r="G79" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H79" t="n">
         <v>2</v>
@@ -6276,7 +6314,7 @@
         <v>-0.01310236048309173</v>
       </c>
       <c r="G80" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H80" t="n">
         <v>3</v>
@@ -6305,7 +6343,7 @@
         <v>-0.008678539752206496</v>
       </c>
       <c r="G81" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H81" t="n">
         <v>3</v>
@@ -6334,7 +6372,7 @@
         <v>-0.004141764801333879</v>
       </c>
       <c r="G82" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H82" t="n">
         <v>3</v>
@@ -6363,7 +6401,7 @@
         <v>1.642574651693381e-05</v>
       </c>
       <c r="G83" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H83" t="n">
         <v>4</v>
@@ -6392,7 +6430,7 @@
         <v>-0.01470502580322882</v>
       </c>
       <c r="G84" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H84" t="n">
         <v>4</v>
@@ -6421,7 +6459,7 @@
         <v>-0.01552034206631986</v>
       </c>
       <c r="G85" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H85" t="n">
         <v>4</v>
@@ -6450,7 +6488,7 @@
         <v>-0.01703554138701916</v>
       </c>
       <c r="G86" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H86" t="n">
         <v>1</v>
@@ -6479,7 +6517,7 @@
         <v>-0.01289961080171436</v>
       </c>
       <c r="G87" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H87" t="n">
         <v>1</v>
@@ -6508,7 +6546,7 @@
         <v>-0.03539719528073028</v>
       </c>
       <c r="G88" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H88" t="n">
         <v>1</v>
@@ -6537,7 +6575,7 @@
         <v>-0.04508011761521417</v>
       </c>
       <c r="G89" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H89" t="n">
         <v>2</v>
@@ -6566,7 +6604,7 @@
         <v>-0.04957830570333151</v>
       </c>
       <c r="G90" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H90" t="n">
         <v>2</v>
@@ -6595,7 +6633,7 @@
         <v>-0.04880070678863985</v>
       </c>
       <c r="G91" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H91" t="n">
         <v>2</v>
@@ -6624,7 +6662,7 @@
         <v>-0.0274894180589785</v>
       </c>
       <c r="G92" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H92" t="n">
         <v>3</v>
@@ -6653,7 +6691,7 @@
         <v>-0.02085837505734224</v>
       </c>
       <c r="G93" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H93" t="n">
         <v>3</v>
@@ -6682,7 +6720,7 @@
         <v>-0.01669978454361145</v>
       </c>
       <c r="G94" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H94" t="n">
         <v>3</v>
@@ -6711,7 +6749,7 @@
         <v>-0.02999219344874965</v>
       </c>
       <c r="G95" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H95" t="n">
         <v>4</v>
@@ -6740,7 +6778,7 @@
         <v>-0.03080314982097817</v>
       </c>
       <c r="G96" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H96" t="n">
         <v>4</v>
@@ -6769,7 +6807,7 @@
         <v>-0.04600766838125035</v>
       </c>
       <c r="G97" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H97" t="n">
         <v>4</v>
@@ -6798,7 +6836,7 @@
         <v>-0.05120162818415125</v>
       </c>
       <c r="G98" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H98" t="n">
         <v>1</v>
@@ -6827,7 +6865,7 @@
         <v>-0.06946387564298999</v>
       </c>
       <c r="G99" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H99" t="n">
         <v>1</v>
@@ -6856,7 +6894,7 @@
         <v>-0.1036546461764051</v>
       </c>
       <c r="G100" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H100" t="n">
         <v>1</v>
@@ -6885,7 +6923,7 @@
         <v>-0.1132003468526878</v>
       </c>
       <c r="G101" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H101" t="n">
         <v>2</v>
@@ -6914,7 +6952,7 @@
         <v>-0.1231526853843904</v>
       </c>
       <c r="G102" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H102" t="n">
         <v>2</v>
@@ -6943,7 +6981,7 @@
         <v>-0.09824854233094853</v>
       </c>
       <c r="G103" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H103" t="n">
         <v>2</v>
@@ -6972,7 +7010,7 @@
         <v>-0.07814990231786137</v>
       </c>
       <c r="G104" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H104" t="n">
         <v>3</v>
@@ -7001,7 +7039,7 @@
         <v>-0.06154336099479781</v>
       </c>
       <c r="G105" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H105" t="n">
         <v>3</v>
@@ -7030,7 +7068,7 @@
         <v>-0.08482641466001017</v>
       </c>
       <c r="G106" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H106" t="n">
         <v>3</v>
@@ -7059,7 +7097,7 @@
         <v>-0.06247971785652189</v>
       </c>
       <c r="G107" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H107" t="n">
         <v>4</v>
@@ -7088,7 +7126,7 @@
         <v>-0.07639133784549447</v>
       </c>
       <c r="G108" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H108" t="n">
         <v>4</v>
@@ -7117,7 +7155,7 @@
         <v>-0.06443636967118098</v>
       </c>
       <c r="G109" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H109" t="n">
         <v>4</v>
@@ -7146,7 +7184,7 @@
         <v>-0.0488799844984841</v>
       </c>
       <c r="G110" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H110" t="n">
         <v>1</v>
@@ -7175,7 +7213,7 @@
         <v>-0.05825045169669583</v>
       </c>
       <c r="G111" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H111" t="n">
         <v>1</v>
@@ -7204,7 +7242,7 @@
         <v>-0.07735581168612655</v>
       </c>
       <c r="G112" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H112" t="n">
         <v>1</v>
@@ -7233,7 +7271,7 @@
         <v>-0.1010225664365227</v>
       </c>
       <c r="G113" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H113" t="n">
         <v>2</v>
@@ -7262,7 +7300,7 @@
         <v>-0.08979818195601069</v>
       </c>
       <c r="G114" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H114" t="n">
         <v>2</v>
@@ -7291,7 +7329,7 @@
         <v>-0.06524048333304372</v>
       </c>
       <c r="G115" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H115" t="n">
         <v>2</v>
@@ -7320,7 +7358,7 @@
         <v>-0.04074387693241805</v>
       </c>
       <c r="G116" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H116" t="n">
         <v>3</v>
@@ -7349,7 +7387,7 @@
         <v>-0.03675707967139325</v>
       </c>
       <c r="G117" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H117" t="n">
         <v>3</v>
@@ -7378,7 +7416,7 @@
         <v>-0.07201037569984288</v>
       </c>
       <c r="G118" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H118" t="n">
         <v>3</v>
@@ -7407,7 +7445,7 @@
         <v>-0.08798764407113459</v>
       </c>
       <c r="G119" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H119" t="n">
         <v>4</v>
@@ -7436,7 +7474,7 @@
         <v>-0.09297937195930114</v>
       </c>
       <c r="G120" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H120" t="n">
         <v>4</v>
@@ -7465,7 +7503,7 @@
         <v>-0.06888446180263902</v>
       </c>
       <c r="G121" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H121" t="n">
         <v>4</v>
@@ -7494,7 +7532,7 @@
         <v>-0.06178402409839879</v>
       </c>
       <c r="G122" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H122" t="n">
         <v>1</v>
@@ -7523,7 +7561,7 @@
         <v>-0.1000963753988781</v>
       </c>
       <c r="G123" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H123" t="n">
         <v>1</v>
@@ -7552,7 +7590,7 @@
         <v>-0.129184632154868</v>
       </c>
       <c r="G124" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H124" t="n">
         <v>1</v>
@@ -7581,7 +7619,7 @@
         <v>-0.1349292609291222</v>
       </c>
       <c r="G125" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H125" t="n">
         <v>2</v>
@@ -7610,7 +7648,7 @@
         <v>-0.1059778059250063</v>
       </c>
       <c r="G126" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H126" t="n">
         <v>2</v>
@@ -7639,7 +7677,7 @@
         <v>-0.081007853314257</v>
       </c>
       <c r="G127" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H127" t="n">
         <v>2</v>
@@ -7668,7 +7706,7 @@
         <v>-0.06182654921614888</v>
       </c>
       <c r="G128" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H128" t="n">
         <v>3</v>
@@ -7697,7 +7735,7 @@
         <v>-0.05965103240997342</v>
       </c>
       <c r="G129" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H129" t="n">
         <v>3</v>
@@ -7726,7 +7764,7 @@
         <v>-0.0903372091951556</v>
       </c>
       <c r="G130" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H130" t="n">
         <v>3</v>
@@ -7755,7 +7793,7 @@
         <v>-0.1209466228210752</v>
       </c>
       <c r="G131" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H131" t="n">
         <v>4</v>
@@ -7784,7 +7822,7 @@
         <v>-0.1459020669822017</v>
       </c>
       <c r="G132" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H132" t="n">
         <v>4</v>
@@ -7813,7 +7851,7 @@
         <v>-0.1448500018406984</v>
       </c>
       <c r="G133" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H133" t="n">
         <v>4</v>
@@ -7842,7 +7880,7 @@
         <v>-0.1655768065392497</v>
       </c>
       <c r="G134" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H134" t="n">
         <v>1</v>
@@ -7871,7 +7909,7 @@
         <v>-0.1688920478560091</v>
       </c>
       <c r="G135" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H135" t="n">
         <v>1</v>
@@ -7900,7 +7938,7 @@
         <v>-0.20286842192788</v>
       </c>
       <c r="G136" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H136" t="n">
         <v>1</v>
@@ -7929,7 +7967,7 @@
         <v>-0.2134075015003669</v>
       </c>
       <c r="G137" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H137" t="n">
         <v>2</v>
@@ -7958,7 +7996,7 @@
         <v>-0.1749832923810191</v>
       </c>
       <c r="G138" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H138" t="n">
         <v>2</v>
@@ -7987,7 +8025,7 @@
         <v>-0.1347935101828394</v>
       </c>
       <c r="G139" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H139" t="n">
         <v>2</v>
@@ -8016,7 +8054,7 @@
         <v>-0.08586343302838688</v>
       </c>
       <c r="G140" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H140" t="n">
         <v>3</v>
@@ -8045,7 +8083,7 @@
         <v>-0.09583413286254644</v>
       </c>
       <c r="G141" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H141" t="n">
         <v>3</v>
@@ -8074,7 +8112,7 @@
         <v>-0.1212332640457878</v>
       </c>
       <c r="G142" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H142" t="n">
         <v>3</v>
@@ -8103,7 +8141,7 @@
         <v>-0.1291033474036325</v>
       </c>
       <c r="G143" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H143" t="n">
         <v>4</v>
@@ -8132,7 +8170,7 @@
         <v>-0.103972413775247</v>
       </c>
       <c r="G144" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H144" t="n">
         <v>4</v>
@@ -8161,7 +8199,7 @@
         <v>-0.1496729265861562</v>
       </c>
       <c r="G145" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H145" t="n">
         <v>4</v>
@@ -8190,7 +8228,7 @@
         <v>-0.1485961495296913</v>
       </c>
       <c r="G146" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H146" t="n">
         <v>1</v>
@@ -8219,7 +8257,7 @@
         <v>-0.1453195655542535</v>
       </c>
       <c r="G147" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H147" t="n">
         <v>1</v>
@@ -8248,7 +8286,7 @@
         <v>-0.1386143662583348</v>
       </c>
       <c r="G148" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H148" t="n">
         <v>1</v>
@@ -8277,7 +8315,7 @@
         <v>-0.1821179183493233</v>
       </c>
       <c r="G149" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H149" t="n">
         <v>2</v>
@@ -8306,7 +8344,7 @@
         <v>-0.1753852982577576</v>
       </c>
       <c r="G150" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H150" t="n">
         <v>2</v>
@@ -8335,7 +8373,7 @@
         <v>-0.1318627511501101</v>
       </c>
       <c r="G151" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H151" t="n">
         <v>2</v>
@@ -8364,7 +8402,7 @@
         <v>-0.1101448680751284</v>
       </c>
       <c r="G152" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H152" t="n">
         <v>3</v>
@@ -8393,7 +8431,7 @@
         <v>-0.1060645126133002</v>
       </c>
       <c r="G153" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H153" t="n">
         <v>3</v>
@@ -8422,7 +8460,7 @@
         <v>-0.1135082142199412</v>
       </c>
       <c r="G154" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H154" t="n">
         <v>3</v>
@@ -8451,7 +8489,7 @@
         <v>-0.1418981805314145</v>
       </c>
       <c r="G155" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H155" t="n">
         <v>4</v>
@@ -8480,7 +8518,7 @@
         <v>-0.1588733260713331</v>
       </c>
       <c r="G156" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H156" t="n">
         <v>4</v>
@@ -8509,7 +8547,7 @@
         <v>-0.1335324447797183</v>
       </c>
       <c r="G157" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H157" t="n">
         <v>4</v>
@@ -8538,7 +8576,7 @@
         <v>-0.1164250865344272</v>
       </c>
       <c r="G158" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H158" t="n">
         <v>1</v>
@@ -8567,7 +8605,7 @@
         <v>-0.09235435026425724</v>
       </c>
       <c r="G159" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H159" t="n">
         <v>1</v>
@@ -8596,7 +8634,7 @@
         <v>-0.1404967846693579</v>
       </c>
       <c r="G160" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="H160" t="n">
         <v>1</v>
@@ -8625,7 +8663,7 @@
         <v>-0.1979602327171737</v>
       </c>
       <c r="G161" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H161" t="n">
         <v>2</v>
@@ -8654,7 +8692,7 @@
         <v>-0.1819517134786032</v>
       </c>
       <c r="G162" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H162" t="n">
         <v>2</v>
@@ -8683,7 +8721,7 @@
         <v>-0.1479617441739821</v>
       </c>
       <c r="G163" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H163" t="n">
         <v>2</v>
@@ -8712,7 +8750,7 @@
         <v>-0.1235469123516771</v>
       </c>
       <c r="G164" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H164" t="n">
         <v>3</v>
@@ -8741,7 +8779,7 @@
         <v>-0.1112892814595854</v>
       </c>
       <c r="G165" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H165" t="n">
         <v>3</v>
@@ -8770,7 +8808,7 @@
         <v>-0.1428458470250424</v>
       </c>
       <c r="G166" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H166" t="n">
         <v>3</v>
@@ -8799,7 +8837,7 @@
         <v>-0.1802221333906949</v>
       </c>
       <c r="G167" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H167" t="n">
         <v>4</v>
@@ -8828,7 +8866,7 @@
         <v>-0.1805484137193039</v>
       </c>
       <c r="G168" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H168" t="n">
         <v>4</v>
@@ -8857,7 +8895,7 @@
         <v>-0.1861102651285657</v>
       </c>
       <c r="G169" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H169" t="n">
         <v>4</v>
@@ -8886,7 +8924,7 @@
         <v>-0.1803040211119578</v>
       </c>
       <c r="G170" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="H170" t="n">
         <v>1</v>
@@ -8915,7 +8953,7 @@
         <v>-0.1566935347558179</v>
       </c>
       <c r="G171" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H171" t="n">
         <v>1</v>
@@ -8944,7 +8982,7 @@
         <v>-0.2201310913406645</v>
       </c>
       <c r="G172" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H172" t="n">
         <v>1</v>
@@ -8973,7 +9011,7 @@
         <v>-0.2635925132742133</v>
       </c>
       <c r="G173" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H173" t="n">
         <v>2</v>
@@ -9002,7 +9040,7 @@
         <v>-0.2131978356272281</v>
       </c>
       <c r="G174" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H174" t="n">
         <v>2</v>
@@ -9031,7 +9069,7 @@
         <v>-0.1607255894791542</v>
       </c>
       <c r="G175" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="H175" t="n">
         <v>2</v>
@@ -9060,7 +9098,7 @@
         <v>-0.1444349165763542</v>
       </c>
       <c r="G176" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H176" t="n">
         <v>3</v>
@@ -9089,7 +9127,7 @@
         <v>-0.1473313183318509</v>
       </c>
       <c r="G177" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H177" t="n">
         <v>3</v>
@@ -9118,7 +9156,7 @@
         <v>-0.1646609371790748</v>
       </c>
       <c r="G178" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H178" t="n">
         <v>3</v>
@@ -9147,7 +9185,7 @@
         <v>-0.21234102942571</v>
       </c>
       <c r="G179" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H179" t="n">
         <v>4</v>
@@ -9176,7 +9214,7 @@
         <v>-0.252829210299896</v>
       </c>
       <c r="G180" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H180" t="n">
         <v>4</v>
@@ -9205,7 +9243,7 @@
         <v>-0.2839536185760727</v>
       </c>
       <c r="G181" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="H181" t="n">
         <v>4</v>
@@ -9234,7 +9272,7 @@
         <v>-0.2400297788304009</v>
       </c>
       <c r="G182" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="H182" t="n">
         <v>1</v>
@@ -9263,7 +9301,7 @@
         <v>-0.2805497954557936</v>
       </c>
       <c r="G183" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H183" t="n">
         <v>1</v>
@@ -9292,7 +9330,7 @@
         <v>-0.3506240564611915</v>
       </c>
       <c r="G184" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H184" t="n">
         <v>1</v>
@@ -9321,7 +9359,7 @@
         <v>-0.3390277903055757</v>
       </c>
       <c r="G185" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H185" t="n">
         <v>2</v>
@@ -9350,7 +9388,7 @@
         <v>-0.3073515739356479</v>
       </c>
       <c r="G186" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H186" t="n">
         <v>2</v>
@@ -9379,7 +9417,7 @@
         <v>-0.2071446270833396</v>
       </c>
       <c r="G187" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H187" t="n">
         <v>2</v>
@@ -9408,7 +9446,7 @@
         <v>-0.1694468249477676</v>
       </c>
       <c r="G188" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="H188" t="n">
         <v>3</v>
@@ -9437,7 +9475,7 @@
         <v>-0.1635296695607648</v>
       </c>
       <c r="G189" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H189" t="n">
         <v>3</v>
@@ -9466,7 +9504,7 @@
         <v>-0.1925750637501429</v>
       </c>
       <c r="G190" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H190" t="n">
         <v>3</v>
@@ -9495,7 +9533,7 @@
         <v>-0.2304897535152396</v>
       </c>
       <c r="G191" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H191" t="n">
         <v>4</v>
@@ -9524,7 +9562,7 @@
         <v>-0.2811118884676824</v>
       </c>
       <c r="G192" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H192" t="n">
         <v>4</v>
@@ -9553,7 +9591,7 @@
         <v>-0.2280847863767602</v>
       </c>
       <c r="G193" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H193" t="n">
         <v>4</v>
@@ -9582,7 +9620,7 @@
         <v>-0.2461641217756053</v>
       </c>
       <c r="G194" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H194" t="n">
         <v>1</v>
@@ -9611,7 +9649,7 @@
         <v>-0.3025532995013631</v>
       </c>
       <c r="G195" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H195" t="n">
         <v>1</v>
@@ -9640,7 +9678,7 @@
         <v>-0.3194948687760681</v>
       </c>
       <c r="G196" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H196" t="n">
         <v>1</v>
@@ -9669,7 +9707,7 @@
         <v>-0.3271115928549875</v>
       </c>
       <c r="G197" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H197" t="n">
         <v>2</v>
@@ -9698,7 +9736,7 @@
         <v>-0.2990789202542029</v>
       </c>
       <c r="G198" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H198" t="n">
         <v>2</v>
@@ -9727,7 +9765,7 @@
         <v>-0.2562999577075886</v>
       </c>
       <c r="G199" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H199" t="n">
         <v>2</v>
@@ -9756,7 +9794,7 @@
         <v>-0.2010680757699633</v>
       </c>
       <c r="G200" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H200" t="n">
         <v>3</v>
@@ -9785,7 +9823,7 @@
         <v>-0.2139935751331455</v>
       </c>
       <c r="G201" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="H201" t="n">
         <v>3</v>
@@ -9814,7 +9852,7 @@
         <v>-0.2482339685577221</v>
       </c>
       <c r="G202" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="H202" t="n">
         <v>3</v>
@@ -9843,7 +9881,7 @@
         <v>-0.2840585191964526</v>
       </c>
       <c r="G203" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H203" t="n">
         <v>4</v>
@@ -9863,22 +9901,22 @@
         <v>309587425.1</v>
       </c>
       <c r="D204" t="n">
-        <v>132144974366.0841</v>
+        <v>132144974396.9284</v>
       </c>
       <c r="E204" t="n">
-        <v>426.8421894829865</v>
+        <v>426.8421895826169</v>
       </c>
       <c r="F204" t="n">
-        <v>-0.2875587826461171</v>
+        <v>-0.2875587824798243</v>
       </c>
       <c r="G204" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="H204" t="n">
         <v>4</v>
       </c>
       <c r="I204" t="n">
-        <v>941.0162909341922</v>
+        <v>941.0162911538373</v>
       </c>
     </row>
     <row r="205" spans="1:9">
@@ -9901,7 +9939,7 @@
         <v>-0.2676784794738392</v>
       </c>
       <c r="G205" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H205" t="n">
         <v>4</v>
@@ -9921,22 +9959,22 @@
         <v>374838323.87</v>
       </c>
       <c r="D206" t="n">
-        <v>170316972745.1041</v>
+        <v>170317037713.1364</v>
       </c>
       <c r="E206" t="n">
-        <v>454.3744913451612</v>
+        <v>454.3746646679731</v>
       </c>
       <c r="F206" t="n">
-        <v>-0.2416046873421802</v>
+        <v>-0.2416043980495138</v>
       </c>
       <c r="G206" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="H206" t="n">
         <v>1</v>
       </c>
       <c r="I206" t="n">
-        <v>1001.714003619542</v>
+        <v>1001.714385727014</v>
       </c>
     </row>
     <row r="207" spans="1:9">
@@ -9950,22 +9988,22 @@
         <v>308647892.4299998</v>
       </c>
       <c r="D207" t="n">
-        <v>123389107676.5222</v>
+        <v>123389159235.4574</v>
       </c>
       <c r="E207" t="n">
-        <v>399.7730446337208</v>
+        <v>399.7732116814684</v>
       </c>
       <c r="F207" t="n">
-        <v>-0.3327398237528988</v>
+        <v>-0.3327395449339264</v>
       </c>
       <c r="G207" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H207" t="n">
         <v>1</v>
       </c>
       <c r="I207" t="n">
-        <v>881.3396541995007</v>
+        <v>881.3400224729652</v>
       </c>
     </row>
     <row r="208" spans="1:9">
@@ -9979,22 +10017,22 @@
         <v>323965391.02</v>
       </c>
       <c r="D208" t="n">
-        <v>125948582910.163</v>
+        <v>125948587003.3804</v>
       </c>
       <c r="E208" t="n">
-        <v>388.7717219225667</v>
+        <v>388.7717345573033</v>
       </c>
       <c r="F208" t="n">
-        <v>-0.3511021036257742</v>
+        <v>-0.3511020825371674</v>
       </c>
       <c r="G208" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H208" t="n">
         <v>1</v>
       </c>
       <c r="I208" t="n">
-        <v>857.0861381504906</v>
+        <v>857.0861660050308</v>
       </c>
     </row>
     <row r="209" spans="1:9">
@@ -10008,22 +10046,22 @@
         <v>303479515.33</v>
       </c>
       <c r="D209" t="n">
-        <v>116144100909.5753</v>
+        <v>116144118683.1379</v>
       </c>
       <c r="E209" t="n">
-        <v>382.708206131414</v>
+        <v>382.7082646973526</v>
       </c>
       <c r="F209" t="n">
-        <v>-0.3612227024750253</v>
+        <v>-0.3612226047227656</v>
       </c>
       <c r="G209" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H209" t="n">
         <v>2</v>
       </c>
       <c r="I209" t="n">
-        <v>843.7185112373152</v>
+        <v>843.7186403517834</v>
       </c>
     </row>
     <row r="210" spans="1:9">
@@ -10046,7 +10084,7 @@
         <v>-0.3244614607886079</v>
       </c>
       <c r="G210" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H210" t="n">
         <v>2</v>
@@ -10066,22 +10104,22 @@
         <v>374930071.58</v>
       </c>
       <c r="D211" t="n">
-        <v>160823730297.2367</v>
+        <v>160826697322.8159</v>
       </c>
       <c r="E211" t="n">
-        <v>428.9432683260277</v>
+        <v>428.9511818699232</v>
       </c>
       <c r="F211" t="n">
-        <v>-0.2840518772708405</v>
+        <v>-0.284038668794768</v>
       </c>
       <c r="G211" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H211" t="n">
         <v>2</v>
       </c>
       <c r="I211" t="n">
-        <v>945.6483293515608</v>
+        <v>945.6657755504327</v>
       </c>
     </row>
     <row r="212" spans="1:9">
@@ -10095,22 +10133,22 @@
         <v>414418886.95</v>
       </c>
       <c r="D212" t="n">
-        <v>190429921330.2875</v>
+        <v>190432602324.1596</v>
       </c>
       <c r="E212" t="n">
-        <v>459.5107204977921</v>
+        <v>459.517189782751</v>
       </c>
       <c r="F212" t="n">
-        <v>-0.2330318202726407</v>
+        <v>-0.2330210224055012</v>
       </c>
       <c r="G212" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H212" t="n">
         <v>3</v>
       </c>
       <c r="I212" t="n">
-        <v>1013.037334409432</v>
+        <v>1013.051596595053</v>
       </c>
     </row>
     <row r="213" spans="1:9">
@@ -10124,22 +10162,22 @@
         <v>411030574.1700001</v>
       </c>
       <c r="D213" t="n">
-        <v>187699928997.2722</v>
+        <v>187702200838.1439</v>
       </c>
       <c r="E213" t="n">
-        <v>456.6568542408245</v>
+        <v>456.6623814230209</v>
       </c>
       <c r="F213" t="n">
-        <v>-0.2377952012138307</v>
+        <v>-0.237785975808026</v>
       </c>
       <c r="G213" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H213" t="n">
         <v>3</v>
       </c>
       <c r="I213" t="n">
-        <v>1006.745700859322</v>
+        <v>1006.757886085192</v>
       </c>
     </row>
     <row r="214" spans="1:9">
@@ -10153,22 +10191,22 @@
         <v>358919294.5599999</v>
       </c>
       <c r="D214" t="n">
-        <v>160445091306.2704</v>
+        <v>160447033886.2697</v>
       </c>
       <c r="E214" t="n">
-        <v>447.0227534102352</v>
+        <v>447.0281657133036</v>
       </c>
       <c r="F214" t="n">
-        <v>-0.2538754545087753</v>
+        <v>-0.2538664208474321</v>
       </c>
       <c r="G214" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="H214" t="n">
         <v>3</v>
       </c>
       <c r="I214" t="n">
-        <v>985.5063621682043</v>
+        <v>985.5182941315492</v>
       </c>
     </row>
     <row r="215" spans="1:9">
@@ -10182,22 +10220,22 @@
         <v>327291940.5099999</v>
       </c>
       <c r="D215" t="n">
-        <v>140860423055.5823</v>
+        <v>140862592745.6425</v>
       </c>
       <c r="E215" t="n">
-        <v>430.3815817648543</v>
+        <v>430.3882109841891</v>
       </c>
       <c r="F215" t="n">
-        <v>-0.2816511919530764</v>
+        <v>-0.2816401271398753</v>
       </c>
       <c r="G215" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H215" t="n">
         <v>4</v>
       </c>
       <c r="I215" t="n">
-        <v>948.8192351587981</v>
+        <v>948.8338499357433</v>
       </c>
     </row>
     <row r="216" spans="1:9">
@@ -10211,22 +10249,22 @@
         <v>324233265.98</v>
       </c>
       <c r="D216" t="n">
-        <v>138151806385.4406</v>
+        <v>138153951422.7566</v>
       </c>
       <c r="E216" t="n">
-        <v>426.0876994464917</v>
+        <v>426.0943151690009</v>
       </c>
       <c r="F216" t="n">
-        <v>-0.2888181000550472</v>
+        <v>-0.2888070577693636</v>
       </c>
       <c r="G216" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H216" t="n">
         <v>4</v>
       </c>
       <c r="I216" t="n">
-        <v>939.3529421997356</v>
+        <v>939.3675272215794</v>
       </c>
     </row>
     <row r="217" spans="1:9">
@@ -10240,22 +10278,22 @@
         <v>343900260.12</v>
       </c>
       <c r="D217" t="n">
-        <v>145880972222.5363</v>
+        <v>145883217662.519</v>
       </c>
       <c r="E217" t="n">
-        <v>424.1955855794725</v>
+        <v>424.2021149144078</v>
       </c>
       <c r="F217" t="n">
-        <v>-0.2919762225181152</v>
+        <v>-0.2919653244217122</v>
       </c>
       <c r="G217" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H217" t="n">
         <v>4</v>
       </c>
       <c r="I217" t="n">
-        <v>935.1815879685053</v>
+        <v>935.1959825403037</v>
       </c>
     </row>
     <row r="218" spans="1:9">
@@ -10269,22 +10307,22 @@
         <v>361391164.43</v>
       </c>
       <c r="D218" t="n">
-        <v>151702277848.1721</v>
+        <v>151704716763.4358</v>
       </c>
       <c r="E218" t="n">
-        <v>419.7730680201958</v>
+        <v>419.7798167055642</v>
       </c>
       <c r="F218" t="n">
-        <v>-0.2993578353748865</v>
+        <v>-0.2993465711612313</v>
       </c>
       <c r="G218" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="H218" t="n">
         <v>1</v>
       </c>
       <c r="I218" t="n">
-        <v>925.4317057573236</v>
+        <v>925.4465839090867</v>
       </c>
     </row>
     <row r="219" spans="1:9">
@@ -10298,22 +10336,22 @@
         <v>317065785.15</v>
       </c>
       <c r="D219" t="n">
-        <v>126198458275.1632</v>
+        <v>126201198620.6871</v>
       </c>
       <c r="E219" t="n">
-        <v>398.0197933228911</v>
+        <v>398.0284361523991</v>
       </c>
       <c r="F219" t="n">
-        <v>-0.3356661710751438</v>
+        <v>-0.3356517453503028</v>
       </c>
       <c r="G219" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H219" t="n">
         <v>1</v>
       </c>
       <c r="I219" t="n">
-        <v>877.4744363596459</v>
+        <v>877.4934903415791</v>
       </c>
     </row>
     <row r="220" spans="1:9">
@@ -10327,22 +10365,22 @@
         <v>329547443.5000001</v>
       </c>
       <c r="D220" t="n">
-        <v>127274375998.3167</v>
+        <v>127277123119.6031</v>
       </c>
       <c r="E220" t="n">
-        <v>386.2095686332238</v>
+        <v>386.2179046750914</v>
       </c>
       <c r="F220" t="n">
-        <v>-0.355378587191557</v>
+        <v>-0.3553646735251893</v>
       </c>
       <c r="G220" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H220" t="n">
         <v>1</v>
       </c>
       <c r="I220" t="n">
-        <v>851.4376150088052</v>
+        <v>851.4559926467067</v>
       </c>
     </row>
     <row r="221" spans="1:9">
@@ -10356,22 +10394,22 @@
         <v>299884009.2</v>
       </c>
       <c r="D221" t="n">
-        <v>104730016902.1645</v>
+        <v>104733686778.1619</v>
       </c>
       <c r="E221" t="n">
-        <v>349.2350831961749</v>
+        <v>349.2473208476831</v>
       </c>
       <c r="F221" t="n">
-        <v>-0.4170926071850151</v>
+        <v>-0.4170721813518787</v>
       </c>
       <c r="G221" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="H221" t="n">
         <v>2</v>
       </c>
       <c r="I221" t="n">
-        <v>769.9236644142874</v>
+        <v>769.9506435408018</v>
       </c>
     </row>
     <row r="222" spans="1:9">
@@ -10385,22 +10423,22 @@
         <v>333948459.15</v>
       </c>
       <c r="D222" t="n">
-        <v>124340565852.5261</v>
+        <v>124344032632.5488</v>
       </c>
       <c r="E222" t="n">
-        <v>372.3345996834677</v>
+        <v>372.344980866335</v>
       </c>
       <c r="F222" t="n">
-        <v>-0.3785372627228696</v>
+        <v>-0.3785199355168393</v>
       </c>
       <c r="G222" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H222" t="n">
         <v>2</v>
       </c>
       <c r="I222" t="n">
-        <v>820.8488584621729</v>
+        <v>820.871744817922</v>
       </c>
     </row>
     <row r="223" spans="1:9">
@@ -10414,22 +10452,22 @@
         <v>356565746.0500001</v>
       </c>
       <c r="D223" t="n">
-        <v>139792283757.903</v>
+        <v>139795777645.5117</v>
       </c>
       <c r="E223" t="n">
-        <v>392.0519155485574</v>
+        <v>392.0617142677203</v>
       </c>
       <c r="F223" t="n">
-        <v>-0.3456271407527558</v>
+        <v>-0.3456107857354191</v>
       </c>
       <c r="G223" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H223" t="n">
         <v>2</v>
       </c>
       <c r="I223" t="n">
-        <v>864.3176530183496</v>
+        <v>864.3392552746164</v>
       </c>
     </row>
     <row r="224" spans="1:9">
@@ -10443,22 +10481,22 @@
         <v>413742056.3300002</v>
       </c>
       <c r="D224" t="n">
-        <v>178872615232.5807</v>
+        <v>178876290872.8297</v>
       </c>
       <c r="E224" t="n">
-        <v>432.3288205681276</v>
+        <v>432.3377044613474</v>
       </c>
       <c r="F224" t="n">
-        <v>-0.278401060598528</v>
+        <v>-0.2783862325148561</v>
       </c>
       <c r="G224" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H224" t="n">
         <v>3</v>
       </c>
       <c r="I224" t="n">
-        <v>953.112117824494</v>
+        <v>953.1317032554864</v>
       </c>
     </row>
     <row r="225" spans="1:9">
@@ -10472,22 +10510,22 @@
         <v>404986271.24</v>
       </c>
       <c r="D225" t="n">
-        <v>173136284930.7256</v>
+        <v>173139508129.842</v>
       </c>
       <c r="E225" t="n">
-        <v>427.5114916873883</v>
+        <v>427.5194504735134</v>
       </c>
       <c r="F225" t="n">
-        <v>-0.2864416520319686</v>
+        <v>-0.2864283680422055</v>
       </c>
       <c r="G225" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H225" t="n">
         <v>3</v>
       </c>
       <c r="I225" t="n">
-        <v>942.4918345740164</v>
+        <v>942.5093805139073</v>
       </c>
     </row>
     <row r="226" spans="1:9">
@@ -10501,22 +10539,22 @@
         <v>363673987.68</v>
       </c>
       <c r="D226" t="n">
-        <v>152681317336.5052</v>
+        <v>152684865189.8102</v>
       </c>
       <c r="E226" t="n">
-        <v>419.8301844751429</v>
+        <v>419.8399400623588</v>
       </c>
       <c r="F226" t="n">
-        <v>-0.2992625024445996</v>
+        <v>-0.2992462194186867</v>
       </c>
       <c r="G226" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H226" t="n">
         <v>3</v>
       </c>
       <c r="I226" t="n">
-        <v>925.5576246939003</v>
+        <v>925.5791318614763</v>
       </c>
     </row>
     <row r="227" spans="1:9">
@@ -10530,22 +10568,22 @@
         <v>323136595.41</v>
       </c>
       <c r="D227" t="n">
-        <v>124381644742.4395</v>
+        <v>124384999437.0709</v>
       </c>
       <c r="E227" t="n">
-        <v>384.919710454405</v>
+        <v>384.9300921155326</v>
       </c>
       <c r="F227" t="n">
-        <v>-0.3575314862108516</v>
+        <v>-0.3575141582065584</v>
       </c>
       <c r="G227" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H227" t="n">
         <v>4</v>
       </c>
       <c r="I227" t="n">
-        <v>848.5939936677813</v>
+        <v>848.6168810779033</v>
       </c>
     </row>
     <row r="228" spans="1:9">
@@ -10559,22 +10597,22 @@
         <v>318034322.98</v>
       </c>
       <c r="D228" t="n">
-        <v>125232926618.4162</v>
+        <v>125236531445.6418</v>
       </c>
       <c r="E228" t="n">
-        <v>393.7717333304668</v>
+        <v>393.7830680417393</v>
       </c>
       <c r="F228" t="n">
-        <v>-0.3427565972489503</v>
+        <v>-0.3427376785110743</v>
       </c>
       <c r="G228" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="H228" t="n">
         <v>4</v>
       </c>
       <c r="I228" t="n">
-        <v>868.1091633003474</v>
+        <v>868.1341518048184</v>
       </c>
     </row>
     <row r="229" spans="1:9">
@@ -10588,22 +10626,22 @@
         <v>340405491.67</v>
       </c>
       <c r="D229" t="n">
-        <v>127425027306.1612</v>
+        <v>127430252029.6028</v>
       </c>
       <c r="E229" t="n">
-        <v>374.3330540321928</v>
+        <v>374.3484025608427</v>
       </c>
       <c r="F229" t="n">
-        <v>-0.3752016476311273</v>
+        <v>-0.3751760294408325</v>
       </c>
       <c r="G229" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="H229" t="n">
         <v>4</v>
       </c>
       <c r="I229" t="n">
-        <v>825.2546509193719</v>
+        <v>825.2884882856339</v>
       </c>
     </row>
     <row r="230" spans="1:9">
@@ -10617,22 +10655,22 @@
         <v>342874144.05</v>
       </c>
       <c r="D230" t="n">
-        <v>122281768373.5009</v>
+        <v>122286035933.623</v>
       </c>
       <c r="E230" t="n">
-        <v>356.6374732405283</v>
+        <v>356.6499196737053</v>
       </c>
       <c r="F230" t="n">
-        <v>-0.4047372967108672</v>
+        <v>-0.404716522400776</v>
       </c>
       <c r="G230" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H230" t="n">
         <v>1</v>
       </c>
       <c r="I230" t="n">
-        <v>786.2429735060688</v>
+        <v>786.2704129126507</v>
       </c>
     </row>
     <row r="231" spans="1:9">
@@ -10646,22 +10684,22 @@
         <v>320542732.65</v>
       </c>
       <c r="D231" t="n">
-        <v>110071422753.0076</v>
+        <v>110075497606.2341</v>
       </c>
       <c r="E231" t="n">
-        <v>343.3907917456808</v>
+        <v>343.403504101356</v>
       </c>
       <c r="F231" t="n">
-        <v>-0.4268472992425276</v>
+        <v>-0.4268260810818683</v>
       </c>
       <c r="G231" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="H231" t="n">
         <v>1</v>
       </c>
       <c r="I231" t="n">
-        <v>757.0393394825279</v>
+        <v>757.0673651418496</v>
       </c>
     </row>
     <row r="232" spans="1:9">
@@ -10675,22 +10713,22 @@
         <v>310837045.06</v>
       </c>
       <c r="D232" t="n">
-        <v>104346654115.9859</v>
+        <v>104351152028.447</v>
       </c>
       <c r="E232" t="n">
-        <v>335.6956829127113</v>
+        <v>335.7101532357714</v>
       </c>
       <c r="F232" t="n">
-        <v>-0.4396911859053522</v>
+        <v>-0.4396670335257833</v>
       </c>
       <c r="G232" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="H232" t="n">
         <v>1</v>
       </c>
       <c r="I232" t="n">
-        <v>740.0747025493636</v>
+        <v>740.1066038235817</v>
       </c>
     </row>
     <row r="233" spans="1:9">
@@ -10704,22 +10742,22 @@
         <v>279802888.0699999</v>
       </c>
       <c r="D233" t="n">
-        <v>87482657952.54382</v>
+        <v>87486749309.2744</v>
       </c>
       <c r="E233" t="n">
-        <v>312.6581664541567</v>
+        <v>312.6727887361453</v>
       </c>
       <c r="F233" t="n">
-        <v>-0.4781430462765655</v>
+        <v>-0.4781186402627339</v>
       </c>
       <c r="G233" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="H233" t="n">
         <v>2</v>
       </c>
       <c r="I233" t="n">
-        <v>689.286193764834</v>
+        <v>689.318430047706</v>
       </c>
     </row>
     <row r="234" spans="1:9">
@@ -10733,22 +10771,22 @@
         <v>308288878.02</v>
       </c>
       <c r="D234" t="n">
-        <v>98040430379.9285</v>
+        <v>98043892288.36937</v>
       </c>
       <c r="E234" t="n">
-        <v>318.0148145778007</v>
+        <v>318.0260440080126</v>
       </c>
       <c r="F234" t="n">
-        <v>-0.4692022784607885</v>
+        <v>-0.4691835354472637</v>
       </c>
       <c r="G234" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H234" t="n">
         <v>2</v>
       </c>
       <c r="I234" t="n">
-        <v>701.0954602182193</v>
+        <v>701.1202166200648</v>
       </c>
     </row>
     <row r="235" spans="1:9">
@@ -10762,22 +10800,22 @@
         <v>356765788.48</v>
       </c>
       <c r="D235" t="n">
-        <v>129485221388.8753</v>
+        <v>129489735373.0206</v>
       </c>
       <c r="E235" t="n">
-        <v>362.941811042328</v>
+        <v>362.9544635563609</v>
       </c>
       <c r="F235" t="n">
-        <v>-0.3942147424536027</v>
+        <v>-0.3941936241744768</v>
       </c>
       <c r="G235" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H235" t="n">
         <v>2</v>
       </c>
       <c r="I235" t="n">
-        <v>800.1415166239165</v>
+        <v>800.1694103563533</v>
       </c>
     </row>
     <row r="236" spans="1:9">
@@ -10791,22 +10829,22 @@
         <v>418415349.29</v>
       </c>
       <c r="D236" t="n">
-        <v>172431311917.3914</v>
+        <v>172439942070.2788</v>
       </c>
       <c r="E236" t="n">
-        <v>412.1056080040714</v>
+        <v>412.126233807838</v>
       </c>
       <c r="F236" t="n">
-        <v>-0.3121555734675443</v>
+        <v>-0.3121211469907187</v>
       </c>
       <c r="G236" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="H236" t="n">
         <v>3</v>
       </c>
       <c r="I236" t="n">
-        <v>908.5280234057758</v>
+        <v>908.5734950527597</v>
       </c>
     </row>
     <row r="237" spans="1:9">
@@ -10820,22 +10858,22 @@
         <v>403364118.94</v>
       </c>
       <c r="D237" t="n">
-        <v>168464177291.7761</v>
+        <v>168480019897.0266</v>
       </c>
       <c r="E237" t="n">
-        <v>417.6479002011455</v>
+        <v>417.6871763898459</v>
       </c>
       <c r="F237" t="n">
-        <v>-0.302904947599007</v>
+        <v>-0.3028393918119264</v>
       </c>
       <c r="G237" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H237" t="n">
         <v>3</v>
       </c>
       <c r="I237" t="n">
-        <v>920.7465607834455</v>
+        <v>920.8331490690545</v>
       </c>
     </row>
     <row r="238" spans="1:9">
@@ -10849,22 +10887,22 @@
         <v>337730785.7099999</v>
       </c>
       <c r="D238" t="n">
-        <v>131357150706.2828</v>
+        <v>131365473955.8737</v>
       </c>
       <c r="E238" t="n">
-        <v>388.9404113105508</v>
+        <v>388.9650559385888</v>
       </c>
       <c r="F238" t="n">
-        <v>-0.350820544595549</v>
+        <v>-0.3507794103093109</v>
       </c>
       <c r="G238" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="H238" t="n">
         <v>3</v>
       </c>
       <c r="I238" t="n">
-        <v>857.4580307752403</v>
+        <v>857.512362322213</v>
       </c>
     </row>
     <row r="239" spans="1:9">
@@ -10878,22 +10916,22 @@
         <v>317001803.61</v>
       </c>
       <c r="D239" t="n">
-        <v>117291187175.753</v>
+        <v>117300334594.4263</v>
       </c>
       <c r="E239" t="n">
-        <v>370.001639864654</v>
+        <v>370.0304959107997</v>
       </c>
       <c r="F239" t="n">
-        <v>-0.3824312000474966</v>
+        <v>-0.3823830364939618</v>
       </c>
       <c r="G239" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H239" t="n">
         <v>4</v>
       </c>
       <c r="I239" t="n">
-        <v>815.7056152456163</v>
+        <v>815.7692312849492</v>
       </c>
     </row>
     <row r="240" spans="1:9">
@@ -10907,22 +10945,22 @@
         <v>305147333.9999999</v>
       </c>
       <c r="D240" t="n">
-        <v>108025155209.2638</v>
+        <v>108030814786.0767</v>
       </c>
       <c r="E240" t="n">
-        <v>354.0098279517127</v>
+        <v>354.0283749818922</v>
       </c>
       <c r="F240" t="n">
-        <v>-0.4091230928070907</v>
+        <v>-0.4090921360059943</v>
       </c>
       <c r="G240" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="H240" t="n">
         <v>4</v>
       </c>
       <c r="I240" t="n">
-        <v>780.4500667023459</v>
+        <v>780.4909554850798</v>
       </c>
     </row>
     <row r="241" spans="1:9">
@@ -10936,22 +10974,22 @@
         <v>347321288.4</v>
       </c>
       <c r="D241" t="n">
-        <v>132232446112.8069</v>
+        <v>132262482607.2273</v>
       </c>
       <c r="E241" t="n">
-        <v>380.7208211220228</v>
+        <v>380.8073015521708</v>
       </c>
       <c r="F241" t="n">
-        <v>-0.3645398417605222</v>
+        <v>-0.3643954974936011</v>
       </c>
       <c r="G241" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="H241" t="n">
         <v>4</v>
       </c>
       <c r="I241" t="n">
-        <v>839.3371222456116</v>
+        <v>839.5277770019158</v>
       </c>
     </row>
     <row r="242" spans="1:9">
@@ -10965,22 +11003,22 @@
         <v>353310194.9999999</v>
       </c>
       <c r="D242" t="n">
-        <v>134206956133.9059</v>
+        <v>134205106923.1703</v>
       </c>
       <c r="E242" t="n">
-        <v>379.8558831111735</v>
+        <v>379.8506491531339</v>
       </c>
       <c r="F242" t="n">
-        <v>-0.3659835076037031</v>
+        <v>-0.3659922435898104</v>
       </c>
       <c r="G242" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="H242" t="n">
         <v>1</v>
       </c>
       <c r="I242" t="n">
-        <v>837.430279906893</v>
+        <v>837.418741122999</v>
       </c>
     </row>
     <row r="243" spans="1:9">
@@ -10994,22 +11032,22 @@
         <v>329568117.91</v>
       </c>
       <c r="D243" t="n">
-        <v>135404241097.6588</v>
+        <v>135402637059.9386</v>
       </c>
       <c r="E243" t="n">
-        <v>410.8535800014357</v>
+        <v>410.8487129113473</v>
       </c>
       <c r="F243" t="n">
-        <v>-0.3142453302355886</v>
+        <v>-0.3142534538833278</v>
       </c>
       <c r="G243" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="H243" t="n">
         <v>1</v>
       </c>
       <c r="I243" t="n">
-        <v>905.7678024711653</v>
+        <v>905.7570724843563</v>
       </c>
     </row>
     <row r="244" spans="1:9">
@@ -11023,22 +11061,109 @@
         <v>314540628.6800001</v>
       </c>
       <c r="D244" t="n">
-        <v>107930501240.0797</v>
+        <v>107934201980.9696</v>
       </c>
       <c r="E244" t="n">
-        <v>343.1369158668639</v>
+        <v>343.1486814085858</v>
       </c>
       <c r="F244" t="n">
-        <v>-0.4272710428288404</v>
+        <v>-0.4272514049929522</v>
       </c>
       <c r="G244" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H244" t="n">
         <v>1</v>
       </c>
       <c r="I244" t="n">
-        <v>756.4796447200882</v>
+        <v>756.5055830333682</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9">
+      <c r="A245" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B245" t="n">
+        <v>4</v>
+      </c>
+      <c r="C245" t="n">
+        <v>296853784.52</v>
+      </c>
+      <c r="D245" t="n">
+        <v>99786583231.6086</v>
+      </c>
+      <c r="E245" t="n">
+        <v>336.1472497073241</v>
+      </c>
+      <c r="F245" t="n">
+        <v>-0.4389374769121992</v>
+      </c>
+      <c r="G245" t="s">
+        <v>335</v>
+      </c>
+      <c r="H245" t="n">
+        <v>2</v>
+      </c>
+      <c r="I245" t="n">
+        <v>741.0702267047667</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9">
+      <c r="A246" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B246" t="n">
+        <v>5</v>
+      </c>
+      <c r="C246" t="n">
+        <v>322319029.37</v>
+      </c>
+      <c r="D246" t="n">
+        <v>113855858220.3395</v>
+      </c>
+      <c r="E246" t="n">
+        <v>353.2396409944533</v>
+      </c>
+      <c r="F246" t="n">
+        <v>-0.4104086099067114</v>
+      </c>
+      <c r="G246" t="s">
+        <v>336</v>
+      </c>
+      <c r="H246" t="n">
+        <v>2</v>
+      </c>
+      <c r="I246" t="n">
+        <v>778.7521125363721</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9">
+      <c r="A247" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B247" t="n">
+        <v>6</v>
+      </c>
+      <c r="C247" t="n">
+        <v>378968470.1699998</v>
+      </c>
+      <c r="D247" t="n">
+        <v>151888514663.7077</v>
+      </c>
+      <c r="E247" t="n">
+        <v>400.7945953803827</v>
+      </c>
+      <c r="F247" t="n">
+        <v>-0.3310347559890441</v>
+      </c>
+      <c r="G247" t="s">
+        <v>337</v>
+      </c>
+      <c r="H247" t="n">
+        <v>2</v>
+      </c>
+      <c r="I247" t="n">
+        <v>883.5917649755918</v>
       </c>
     </row>
   </sheetData>

</xml_diff>